<commit_message>
added new task Meeting Minutes Wiki
</commit_message>
<xml_diff>
--- a/docs/Tasks List.xlsx
+++ b/docs/Tasks List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="74">
   <si>
     <t>Task</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>GUI Tests/Cont do</t>
+  </si>
+  <si>
+    <t>Meeting Minutes Wiki</t>
   </si>
 </sst>
 </file>
@@ -480,24 +483,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -525,6 +510,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -536,6 +539,97 @@
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="36">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Century Gothic"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Century Gothic"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -562,97 +656,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Century Gothic"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Century Gothic"/>
-        <scheme val="major"/>
-      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1158,20 +1161,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ToDoList" displayName="ToDoList" ref="B4:J46" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="B4:J46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ToDoList" displayName="ToDoList" ref="B4:J47" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="B4:J47"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Task" dataDxfId="17"/>
-    <tableColumn id="2" name="Main Responsibility" dataDxfId="0"/>
-    <tableColumn id="3" name="Priority " dataDxfId="16"/>
-    <tableColumn id="4" name="Status " dataDxfId="15"/>
-    <tableColumn id="6" name="Start Date " dataDxfId="14"/>
-    <tableColumn id="7" name="Due Date " dataDxfId="13"/>
-    <tableColumn id="5" name="% Complete" dataDxfId="12"/>
-    <tableColumn id="9" name="Done/Overdue?" dataDxfId="11">
+    <tableColumn id="1" name="Task" dataDxfId="19"/>
+    <tableColumn id="2" name="Main Responsibility" dataDxfId="18"/>
+    <tableColumn id="3" name="Priority " dataDxfId="17"/>
+    <tableColumn id="4" name="Status " dataDxfId="16"/>
+    <tableColumn id="6" name="Start Date " dataDxfId="15"/>
+    <tableColumn id="7" name="Due Date " dataDxfId="14"/>
+    <tableColumn id="5" name="% Complete" dataDxfId="13"/>
+    <tableColumn id="9" name="Done/Overdue?" dataDxfId="12">
       <calculatedColumnFormula>IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Notes" dataDxfId="1"/>
+    <tableColumn id="10" name="Notes" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1183,20 +1186,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ToDoList2" displayName="ToDoList2" ref="B4:J9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ToDoList2" displayName="ToDoList2" ref="B4:J9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="B4:J9"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Task" dataDxfId="10"/>
-    <tableColumn id="2" name="Main Responsibility" dataDxfId="9"/>
-    <tableColumn id="3" name="Priority " dataDxfId="8"/>
-    <tableColumn id="4" name="Status " dataDxfId="7"/>
-    <tableColumn id="6" name="Start Date " dataDxfId="6"/>
-    <tableColumn id="7" name="Due Date " dataDxfId="5"/>
-    <tableColumn id="5" name="% Complete" dataDxfId="4"/>
-    <tableColumn id="9" name="Done/Overdue?" dataDxfId="3">
+    <tableColumn id="1" name="Task" dataDxfId="8"/>
+    <tableColumn id="2" name="Main Responsibility" dataDxfId="7"/>
+    <tableColumn id="3" name="Priority " dataDxfId="6"/>
+    <tableColumn id="4" name="Status " dataDxfId="5"/>
+    <tableColumn id="6" name="Start Date " dataDxfId="4"/>
+    <tableColumn id="7" name="Due Date " dataDxfId="3"/>
+    <tableColumn id="5" name="% Complete" dataDxfId="2"/>
+    <tableColumn id="9" name="Done/Overdue?" dataDxfId="1">
       <calculatedColumnFormula>IF(AND(ToDoList2[[#This Row],[Status ]]="Complete",ToDoList2[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList2[[#This Row],[Due Date ]]),2,IF(AND(ToDoList2[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList2[[#This Row],[Due Date ]]),3,2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Notes" dataDxfId="2"/>
+    <tableColumn id="10" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="To Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1448,23 +1451,23 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J46"/>
+  <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.36328125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" style="18" customWidth="1"/>
     <col min="4" max="4" width="11.90625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.26953125" style="1" customWidth="1"/>
     <col min="6" max="7" width="16.7265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.7265625" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.26953125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7265625" style="24" customWidth="1"/>
+    <col min="10" max="10" width="30.7265625" style="18" customWidth="1"/>
     <col min="11" max="11" width="2.81640625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="8.81640625" style="1"/>
   </cols>
@@ -1476,7 +1479,7 @@
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -1497,7 +1500,7 @@
       <c r="I4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1505,7 +1508,7 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1525,13 +1528,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J5" s="26"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1551,13 +1554,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J6" s="26"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1577,13 +1580,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1605,13 +1608,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="J8" s="26"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1631,7 +1634,7 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="20" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1639,7 +1642,7 @@
       <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1659,7 +1662,7 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="21" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1667,7 +1670,7 @@
       <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1689,13 +1692,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="J11" s="27"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1717,13 +1720,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1745,13 +1748,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="J13" s="27"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1771,7 +1774,7 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="21" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1779,7 +1782,7 @@
       <c r="B15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1799,13 +1802,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J15" s="27"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1825,13 +1828,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J16" s="27"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1851,13 +1854,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J17" s="27"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -1877,13 +1880,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J18" s="27"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1903,13 +1906,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J19" s="27"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1927,13 +1930,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J20" s="27"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="29"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1951,13 +1954,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="29"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="4" t="s">
         <v>7</v>
       </c>
@@ -1975,13 +1978,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J22" s="27"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="29"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="4" t="s">
         <v>7</v>
       </c>
@@ -1999,13 +2002,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J23" s="27"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="29"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
@@ -2023,13 +2026,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J24" s="27"/>
+      <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="29"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="4" t="s">
         <v>7</v>
       </c>
@@ -2047,13 +2050,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J25" s="27"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="29"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
@@ -2071,13 +2074,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J26" s="27"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="29"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
@@ -2095,13 +2098,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J27" s="27"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="29"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
@@ -2119,13 +2122,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J28" s="27"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="29"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
@@ -2143,13 +2146,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J29" s="27"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="29"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
@@ -2167,13 +2170,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J30" s="27"/>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="29"/>
+      <c r="C31" s="23"/>
       <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
@@ -2191,13 +2194,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J31" s="27"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="29"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
@@ -2215,13 +2218,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J32" s="27"/>
+      <c r="J32" s="21"/>
     </row>
     <row r="33" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="29"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="4" t="s">
         <v>7</v>
       </c>
@@ -2239,13 +2242,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J33" s="27"/>
+      <c r="J33" s="21"/>
     </row>
     <row r="34" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="29"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="4" t="s">
         <v>7</v>
       </c>
@@ -2263,13 +2266,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J34" s="27"/>
+      <c r="J34" s="21"/>
     </row>
     <row r="35" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="29"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="4" t="s">
         <v>7</v>
       </c>
@@ -2287,13 +2290,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J35" s="27"/>
+      <c r="J35" s="21"/>
     </row>
     <row r="36" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="29"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="4" t="s">
         <v>7</v>
       </c>
@@ -2311,13 +2314,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J36" s="27"/>
+      <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="29"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="4" t="s">
         <v>7</v>
       </c>
@@ -2335,7 +2338,7 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J37" s="27" t="s">
+      <c r="J37" s="21" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2343,7 +2346,7 @@
       <c r="B38" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="29"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="4" t="s">
         <v>7</v>
       </c>
@@ -2361,13 +2364,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J38" s="27"/>
+      <c r="J38" s="21"/>
     </row>
     <row r="39" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="29"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="4" t="s">
         <v>7</v>
       </c>
@@ -2385,13 +2388,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J39" s="27"/>
+      <c r="J39" s="21"/>
     </row>
     <row r="40" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="29"/>
+      <c r="C40" s="23"/>
       <c r="D40" s="4" t="s">
         <v>7</v>
       </c>
@@ -2409,13 +2412,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J40" s="27"/>
+      <c r="J40" s="21"/>
     </row>
     <row r="41" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="29"/>
+      <c r="C41" s="23"/>
       <c r="D41" s="4" t="s">
         <v>7</v>
       </c>
@@ -2433,13 +2436,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J41" s="27"/>
+      <c r="J41" s="21"/>
     </row>
     <row r="42" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="29"/>
+      <c r="C42" s="23"/>
       <c r="D42" s="4" t="s">
         <v>7</v>
       </c>
@@ -2457,13 +2460,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J42" s="27"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2485,13 +2488,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="J43" s="27"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="23"/>
       <c r="D44" s="6" t="s">
         <v>7</v>
       </c>
@@ -2507,13 +2510,13 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J44" s="27"/>
+      <c r="J44" s="21"/>
     </row>
     <row r="45" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2535,7 +2538,7 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>1</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="J45" s="21" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2543,7 +2546,7 @@
       <c r="B46" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="30"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="12"/>
@@ -2555,10 +2558,32 @@
         <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
         <v>2</v>
       </c>
-      <c r="J46" s="27"/>
+      <c r="J46" s="21"/>
+    </row>
+    <row r="47" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="23"/>
+      <c r="D47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="12"/>
+      <c r="G47" s="8">
+        <v>42286</v>
+      </c>
+      <c r="H47" s="13"/>
+      <c r="I47" s="10">
+        <f ca="1">IF(AND(ToDoList[[#This Row],[Status ]]="Complete",ToDoList[[#This Row],[% Complete]]=1),1,IF(ISBLANK(ToDoList[[#This Row],[Due Date ]]),2,IF(AND(ToDoList[[#This Row],[Status ]]&lt;&gt;"Complete",TODAY()&gt;ToDoList[[#This Row],[Due Date ]]),3,2)))</f>
+        <v>2</v>
+      </c>
+      <c r="J47" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8IRRYAoh3j7M46A/RtG6N+1AnO5mehQ452WQPzYa41xvFuTvhIQL1WvtUpSNA8f0vLuHUjLV6UWG3wkTqLiIUQ==" saltValue="60hCGIS27Y25lrOaJ3HhLA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="yFl4pkAGMp8G9ZShY4zauE++zsWEe1FIptr0Pr/zfrrhFhFeaUzKUu9iiCmWhmIb+VjIlt8JaS1RJwMMHIKaaQ==" saltValue="oEdqjBr6gRLLYlNnld9SJw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H5:H10 H14:H46">
     <cfRule type="dataBar" priority="60">
@@ -2617,19 +2642,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="E5:E46">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly you need to select a choice from the drop down list. But you can still use what you entered by clicking Yes." sqref="E5:E47">
       <formula1>"Not Started,In Progress, Deferred, Complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H5:H46">
+    <dataValidation type="list" allowBlank="1" sqref="H5:H47">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="D5:D46">
+    <dataValidation type="list" allowBlank="1" errorTitle="Whoops" sqref="D5:D47">
       <formula1>"Low, Normal, High"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="G5:G46">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops" error="For this template to work correctly, your Due Date needs to be greater than or equal to the Start Date." sqref="G5:G47">
       <formula1>G5&gt;=F5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C46">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C47">
       <formula1>Team_Members</formula1>
     </dataValidation>
   </dataValidations>
@@ -2711,7 +2736,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I5:I46</xm:sqref>
+          <xm:sqref>I5:I47</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2912,76 +2937,76 @@
       <c r="B13" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>1</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17">
         <v>2</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
     </row>
     <row r="16" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
         <v>3</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>4</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
     </row>
     <row r="19" spans="2:10" ht="26" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Jake is done his part
</commit_message>
<xml_diff>
--- a/docs/Tasks List.xlsx
+++ b/docs/Tasks List.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="74">
   <si>
     <t>Task</t>
   </si>
@@ -254,8 +254,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -369,7 +370,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -409,19 +410,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
       <protection locked="0"/>
@@ -449,6 +441,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -546,7 +550,7 @@
       <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>31680</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>3960</xdr:rowOff>
@@ -606,13 +610,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>855720</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>48240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1541160</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>918360</xdr:rowOff>
@@ -1100,10 +1104,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK47"/>
+  <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1113,48 +1117,45 @@
     <col min="3" max="3" width="21.453125" style="2"/>
     <col min="4" max="4" width="11.81640625" style="1"/>
     <col min="5" max="5" width="18.26953125" style="1"/>
-    <col min="6" max="7" width="16.7265625" style="1"/>
+    <col min="6" max="6" width="16.7265625" style="25"/>
+    <col min="7" max="7" width="16.7265625" style="1"/>
     <col min="8" max="8" width="18.7265625" style="1"/>
-    <col min="9" max="9" width="20.26953125" style="1"/>
-    <col min="10" max="10" width="30.7265625" style="2"/>
-    <col min="11" max="11" width="2.81640625" style="1"/>
-    <col min="12" max="1025" width="8.81640625" style="1"/>
+    <col min="9" max="9" width="30.7265625" style="2"/>
+    <col min="10" max="10" width="2.81640625" style="1"/>
+    <col min="11" max="1024" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1"/>
+      <c r="F1" s="22"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="2:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2"/>
+      <c r="F2" s="22"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="2:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
-      <c r="F3"/>
+      <c r="F3" s="22"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1168,7 @@
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1176,14 +1177,11 @@
       <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1196,20 +1194,16 @@
       <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="5">
         <v>42286</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
       </c>
-      <c r="I5" s="7" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1222,20 +1216,16 @@
       <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="5">
         <v>42286</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
       </c>
-      <c r="I6" s="8" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1248,20 +1238,16 @@
       <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="5">
         <v>42286</v>
       </c>
       <c r="H7" s="6">
         <v>0</v>
       </c>
-      <c r="I7" s="8" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1274,7 +1260,7 @@
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="23">
         <v>42282</v>
       </c>
       <c r="G8" s="5">
@@ -1283,13 +1269,9 @@
       <c r="H8" s="6">
         <v>1</v>
       </c>
-      <c r="I8" s="8" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1302,22 +1284,18 @@
       <c r="E9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="5">
         <v>42286</v>
       </c>
       <c r="H9" s="6">
         <v>0</v>
       </c>
-      <c r="I9" s="8" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
@@ -1330,22 +1308,18 @@
       <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="5">
         <v>42286</v>
       </c>
       <c r="H10" s="6">
         <v>0</v>
       </c>
-      <c r="I10" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
@@ -1358,7 +1332,7 @@
       <c r="E11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="23">
         <v>42282</v>
       </c>
       <c r="G11" s="5">
@@ -1367,13 +1341,9 @@
       <c r="H11" s="6">
         <v>1</v>
       </c>
-      <c r="I11" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>22</v>
       </c>
@@ -1386,7 +1356,7 @@
       <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="23">
         <v>42282</v>
       </c>
       <c r="G12" s="5">
@@ -1395,13 +1365,9 @@
       <c r="H12" s="6">
         <v>1</v>
       </c>
-      <c r="I12" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>23</v>
       </c>
@@ -1414,7 +1380,7 @@
       <c r="E13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="23">
         <v>42282</v>
       </c>
       <c r="G13" s="5">
@@ -1423,13 +1389,9 @@
       <c r="H13" s="6">
         <v>1</v>
       </c>
-      <c r="I13" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>24</v>
       </c>
@@ -1442,26 +1404,22 @@
       <c r="E14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="5">
         <v>42286</v>
       </c>
       <c r="H14" s="6">
         <v>0</v>
       </c>
-      <c r="I14" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" s="14" t="s">
+      <c r="I14" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1470,24 +1428,20 @@
       <c r="E15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="5">
         <v>42286</v>
       </c>
       <c r="H15" s="6">
         <v>0</v>
       </c>
-      <c r="I15" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1496,24 +1450,20 @@
       <c r="E16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="5">
         <v>42286</v>
       </c>
       <c r="H16" s="6">
         <v>0</v>
       </c>
-      <c r="I16" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1522,24 +1472,20 @@
       <c r="E17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="5">
         <v>42286</v>
       </c>
       <c r="H17" s="6">
         <v>0</v>
       </c>
-      <c r="I17" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1548,24 +1494,20 @@
       <c r="E18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="5">
         <v>42286</v>
       </c>
       <c r="H18" s="6">
         <v>0</v>
       </c>
-      <c r="I18" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1574,336 +1516,280 @@
       <c r="E19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="15"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="5">
         <v>42286</v>
       </c>
       <c r="H19" s="6">
         <v>0</v>
       </c>
-      <c r="I19" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="15"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="5">
         <v>42286</v>
       </c>
       <c r="H20" s="6">
         <v>0</v>
       </c>
-      <c r="I20" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="16"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="5">
         <v>42286</v>
       </c>
       <c r="H21" s="6">
         <v>0</v>
       </c>
-      <c r="I21" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="5">
         <v>42286</v>
       </c>
       <c r="H22" s="6">
         <v>0</v>
       </c>
-      <c r="I22" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="15"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="5">
         <v>42286</v>
       </c>
       <c r="H23" s="6">
         <v>0</v>
       </c>
-      <c r="I23" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="5">
         <v>42286</v>
       </c>
       <c r="H24" s="6">
         <v>0</v>
       </c>
-      <c r="I24" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="16"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="5">
         <v>42286</v>
       </c>
       <c r="H25" s="6">
         <v>0</v>
       </c>
-      <c r="I25" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="15"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="5">
         <v>42286</v>
       </c>
       <c r="H26" s="6">
         <v>0</v>
       </c>
-      <c r="I26" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="15"/>
+      <c r="F27" s="24"/>
       <c r="G27" s="5">
         <v>42286</v>
       </c>
       <c r="H27" s="6">
         <v>0</v>
       </c>
-      <c r="I27" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="16"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="15"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="5">
         <v>42286</v>
       </c>
       <c r="H28" s="6">
         <v>0</v>
       </c>
-      <c r="I28" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="15"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="5">
         <v>42286</v>
       </c>
       <c r="H29" s="6">
         <v>0</v>
       </c>
-      <c r="I29" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J29" s="14"/>
-    </row>
-    <row r="30" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="15"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="5">
         <v>42286</v>
       </c>
       <c r="H30" s="6">
         <v>0</v>
       </c>
-      <c r="I30" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J30" s="14"/>
-    </row>
-    <row r="31" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="16"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="15"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="5">
         <v>42286</v>
       </c>
       <c r="H31" s="6">
         <v>0</v>
       </c>
-      <c r="I31" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J31" s="14"/>
-    </row>
-    <row r="32" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="15"/>
+      <c r="F32" s="24"/>
       <c r="G32" s="5">
         <v>42286</v>
       </c>
       <c r="H32" s="6">
         <v>0</v>
       </c>
-      <c r="I32" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J32" s="14"/>
-    </row>
-    <row r="33" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -1912,24 +1798,20 @@
       <c r="E33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="15"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="5">
         <v>42286</v>
       </c>
       <c r="H33" s="6">
         <v>0</v>
       </c>
-      <c r="I33" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -1938,24 +1820,20 @@
       <c r="E34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="15"/>
+      <c r="F34" s="24"/>
       <c r="G34" s="5">
         <v>42286</v>
       </c>
       <c r="H34" s="6">
         <v>0</v>
       </c>
-      <c r="I34" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J34" s="14"/>
-    </row>
-    <row r="35" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -1964,24 +1842,20 @@
       <c r="E35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="15"/>
+      <c r="F35" s="24"/>
       <c r="G35" s="5">
         <v>42286</v>
       </c>
       <c r="H35" s="6">
         <v>0</v>
       </c>
-      <c r="I35" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J35" s="14"/>
-    </row>
-    <row r="36" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -1990,24 +1864,20 @@
       <c r="E36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="15"/>
+      <c r="F36" s="24"/>
       <c r="G36" s="5">
         <v>42286</v>
       </c>
       <c r="H36" s="6">
         <v>0</v>
       </c>
-      <c r="I36" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J36" s="14"/>
-    </row>
-    <row r="37" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -2016,152 +1886,134 @@
       <c r="E37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="15"/>
+      <c r="F37" s="24"/>
       <c r="G37" s="5">
         <v>42286</v>
       </c>
       <c r="H37" s="6">
         <v>0</v>
       </c>
-      <c r="I37" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J37" s="14" t="s">
+      <c r="I37" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="13" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="15"/>
+        <v>17</v>
+      </c>
+      <c r="F38" s="24">
+        <v>42284</v>
+      </c>
       <c r="G38" s="5">
         <v>42286</v>
       </c>
       <c r="H38" s="6">
-        <v>0</v>
-      </c>
-      <c r="I38" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J38" s="14"/>
-    </row>
-    <row r="39" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="13" t="s">
         <v>73</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="15"/>
+        <v>17</v>
+      </c>
+      <c r="F39" s="24">
+        <v>42284</v>
+      </c>
       <c r="G39" s="5">
         <v>42286</v>
       </c>
       <c r="H39" s="6">
-        <v>0</v>
-      </c>
-      <c r="I39" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J39" s="14"/>
-    </row>
-    <row r="40" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="13" t="s">
         <v>73</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="15"/>
+        <v>17</v>
+      </c>
+      <c r="F40" s="24">
+        <v>42284</v>
+      </c>
       <c r="G40" s="5">
         <v>42286</v>
       </c>
       <c r="H40" s="6">
-        <v>0</v>
-      </c>
-      <c r="I40" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J40" s="14"/>
-    </row>
-    <row r="41" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="16"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="15"/>
+      <c r="F41" s="24"/>
       <c r="G41" s="5">
         <v>42286</v>
       </c>
       <c r="H41" s="6">
         <v>0</v>
       </c>
-      <c r="I41" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J41" s="14"/>
-    </row>
-    <row r="42" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="16"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="15"/>
+      <c r="F42" s="24"/>
       <c r="G42" s="5">
         <v>42286</v>
       </c>
       <c r="H42" s="6">
         <v>0</v>
       </c>
-      <c r="I42" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J42" s="14"/>
-    </row>
-    <row r="43" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="13" t="s">
         <v>53</v>
       </c>
       <c r="D43" s="11" t="s">
@@ -2170,7 +2022,7 @@
       <c r="E43" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="15">
+      <c r="F43" s="24">
         <v>42282</v>
       </c>
       <c r="G43" s="5">
@@ -2179,41 +2031,33 @@
       <c r="H43" s="6">
         <v>1</v>
       </c>
-      <c r="I43" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J43" s="14"/>
-    </row>
-    <row r="44" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="15"/>
+      <c r="F44" s="24"/>
       <c r="G44" s="5">
         <v>42288</v>
       </c>
       <c r="H44" s="6">
         <v>0</v>
       </c>
-      <c r="I44" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J44" s="14"/>
-    </row>
-    <row r="45" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D45" s="11" t="s">
@@ -2222,7 +2066,7 @@
       <c r="E45" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F45" s="15">
+      <c r="F45" s="24">
         <v>42282</v>
       </c>
       <c r="G45" s="5">
@@ -2231,39 +2075,31 @@
       <c r="H45" s="6">
         <v>1</v>
       </c>
-      <c r="I45" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J45" s="14" t="s">
+      <c r="I45" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
-      <c r="F46" s="15"/>
+      <c r="F46" s="24"/>
       <c r="G46" s="5">
         <v>42286</v>
       </c>
-      <c r="H46" s="17"/>
-      <c r="I46" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="14"/>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -2272,19 +2108,14 @@
       <c r="E47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="15"/>
+      <c r="F47" s="24"/>
       <c r="G47" s="5">
         <v>42286</v>
       </c>
-      <c r="H47" s="17"/>
-      <c r="I47" s="13" t="e">
-        <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="H12">
     <cfRule type="dataBar" priority="3">
       <dataBar>
@@ -2351,11 +2182,11 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -2406,7 +2237,7 @@
   <dimension ref="A1:AMK19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2594,7 +2425,7 @@
       <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2650,79 +2481,79 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20">
+      <c r="B14" s="17">
         <v>1</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21">
+      <c r="B15" s="18">
         <v>2</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20">
+      <c r="B16" s="17">
         <v>3</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21">
+      <c r="B17" s="18">
         <v>4</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="19" spans="2:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
time travel is fun, excel
</commit_message>
<xml_diff>
--- a/docs/Tasks List.xlsx
+++ b/docs/Tasks List.xlsx
@@ -297,7 +297,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +314,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCE3E6"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -370,7 +376,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -402,10 +408,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -453,6 +455,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1106,8 +1144,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1155,7 @@
     <col min="3" max="3" width="21.453125" style="2"/>
     <col min="4" max="4" width="11.81640625" style="1"/>
     <col min="5" max="5" width="18.26953125" style="1"/>
-    <col min="6" max="6" width="16.7265625" style="22"/>
+    <col min="6" max="6" width="16.7265625" style="21"/>
     <col min="7" max="7" width="16.7265625" style="1"/>
     <col min="8" max="8" width="18.7265625" style="1"/>
     <col min="9" max="9" width="30.7265625" style="2"/>
@@ -1125,37 +1163,37 @@
     <col min="11" max="1024" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1" s="19"/>
+      <c r="F1" s="18"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="2:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2" s="19"/>
+      <c r="F2" s="18"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
     </row>
-    <row r="3" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
-      <c r="F3" s="19"/>
+      <c r="F3" s="18"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1206,7 @@
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1181,7 +1219,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1194,16 +1232,18 @@
       <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19">
+        <v>42282</v>
+      </c>
       <c r="G5" s="5">
         <v>42286</v>
       </c>
       <c r="H5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1216,16 +1256,18 @@
       <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19">
+        <v>42282</v>
+      </c>
       <c r="G6" s="5">
         <v>42286</v>
       </c>
       <c r="H6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1238,16 +1280,18 @@
       <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="19">
+        <v>42282</v>
+      </c>
       <c r="G7" s="5">
         <v>42286</v>
       </c>
       <c r="H7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1260,7 +1304,7 @@
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="19">
         <v>42282</v>
       </c>
       <c r="G8" s="5">
@@ -1271,56 +1315,2088 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:1024" s="32" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="5">
+      <c r="F9" s="28"/>
+      <c r="G9" s="29">
         <v>42286</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="30">
         <v>0</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="31" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AD9" s="25"/>
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="25"/>
+      <c r="AJ9" s="25"/>
+      <c r="AK9" s="25"/>
+      <c r="AL9" s="25"/>
+      <c r="AM9" s="25"/>
+      <c r="AN9" s="25"/>
+      <c r="AO9" s="25"/>
+      <c r="AP9" s="25"/>
+      <c r="AQ9" s="25"/>
+      <c r="AR9" s="25"/>
+      <c r="AS9" s="25"/>
+      <c r="AT9" s="25"/>
+      <c r="AU9" s="25"/>
+      <c r="AV9" s="25"/>
+      <c r="AW9" s="25"/>
+      <c r="AX9" s="25"/>
+      <c r="AY9" s="25"/>
+      <c r="AZ9" s="25"/>
+      <c r="BA9" s="25"/>
+      <c r="BB9" s="25"/>
+      <c r="BC9" s="25"/>
+      <c r="BD9" s="25"/>
+      <c r="BE9" s="25"/>
+      <c r="BF9" s="25"/>
+      <c r="BG9" s="25"/>
+      <c r="BH9" s="25"/>
+      <c r="BI9" s="25"/>
+      <c r="BJ9" s="25"/>
+      <c r="BK9" s="25"/>
+      <c r="BL9" s="25"/>
+      <c r="BM9" s="25"/>
+      <c r="BN9" s="25"/>
+      <c r="BO9" s="25"/>
+      <c r="BP9" s="25"/>
+      <c r="BQ9" s="25"/>
+      <c r="BR9" s="25"/>
+      <c r="BS9" s="25"/>
+      <c r="BT9" s="25"/>
+      <c r="BU9" s="25"/>
+      <c r="BV9" s="25"/>
+      <c r="BW9" s="25"/>
+      <c r="BX9" s="25"/>
+      <c r="BY9" s="25"/>
+      <c r="BZ9" s="25"/>
+      <c r="CA9" s="25"/>
+      <c r="CB9" s="25"/>
+      <c r="CC9" s="25"/>
+      <c r="CD9" s="25"/>
+      <c r="CE9" s="25"/>
+      <c r="CF9" s="25"/>
+      <c r="CG9" s="25"/>
+      <c r="CH9" s="25"/>
+      <c r="CI9" s="25"/>
+      <c r="CJ9" s="25"/>
+      <c r="CK9" s="25"/>
+      <c r="CL9" s="25"/>
+      <c r="CM9" s="25"/>
+      <c r="CN9" s="25"/>
+      <c r="CO9" s="25"/>
+      <c r="CP9" s="25"/>
+      <c r="CQ9" s="25"/>
+      <c r="CR9" s="25"/>
+      <c r="CS9" s="25"/>
+      <c r="CT9" s="25"/>
+      <c r="CU9" s="25"/>
+      <c r="CV9" s="25"/>
+      <c r="CW9" s="25"/>
+      <c r="CX9" s="25"/>
+      <c r="CY9" s="25"/>
+      <c r="CZ9" s="25"/>
+      <c r="DA9" s="25"/>
+      <c r="DB9" s="25"/>
+      <c r="DC9" s="25"/>
+      <c r="DD9" s="25"/>
+      <c r="DE9" s="25"/>
+      <c r="DF9" s="25"/>
+      <c r="DG9" s="25"/>
+      <c r="DH9" s="25"/>
+      <c r="DI9" s="25"/>
+      <c r="DJ9" s="25"/>
+      <c r="DK9" s="25"/>
+      <c r="DL9" s="25"/>
+      <c r="DM9" s="25"/>
+      <c r="DN9" s="25"/>
+      <c r="DO9" s="25"/>
+      <c r="DP9" s="25"/>
+      <c r="DQ9" s="25"/>
+      <c r="DR9" s="25"/>
+      <c r="DS9" s="25"/>
+      <c r="DT9" s="25"/>
+      <c r="DU9" s="25"/>
+      <c r="DV9" s="25"/>
+      <c r="DW9" s="25"/>
+      <c r="DX9" s="25"/>
+      <c r="DY9" s="25"/>
+      <c r="DZ9" s="25"/>
+      <c r="EA9" s="25"/>
+      <c r="EB9" s="25"/>
+      <c r="EC9" s="25"/>
+      <c r="ED9" s="25"/>
+      <c r="EE9" s="25"/>
+      <c r="EF9" s="25"/>
+      <c r="EG9" s="25"/>
+      <c r="EH9" s="25"/>
+      <c r="EI9" s="25"/>
+      <c r="EJ9" s="25"/>
+      <c r="EK9" s="25"/>
+      <c r="EL9" s="25"/>
+      <c r="EM9" s="25"/>
+      <c r="EN9" s="25"/>
+      <c r="EO9" s="25"/>
+      <c r="EP9" s="25"/>
+      <c r="EQ9" s="25"/>
+      <c r="ER9" s="25"/>
+      <c r="ES9" s="25"/>
+      <c r="ET9" s="25"/>
+      <c r="EU9" s="25"/>
+      <c r="EV9" s="25"/>
+      <c r="EW9" s="25"/>
+      <c r="EX9" s="25"/>
+      <c r="EY9" s="25"/>
+      <c r="EZ9" s="25"/>
+      <c r="FA9" s="25"/>
+      <c r="FB9" s="25"/>
+      <c r="FC9" s="25"/>
+      <c r="FD9" s="25"/>
+      <c r="FE9" s="25"/>
+      <c r="FF9" s="25"/>
+      <c r="FG9" s="25"/>
+      <c r="FH9" s="25"/>
+      <c r="FI9" s="25"/>
+      <c r="FJ9" s="25"/>
+      <c r="FK9" s="25"/>
+      <c r="FL9" s="25"/>
+      <c r="FM9" s="25"/>
+      <c r="FN9" s="25"/>
+      <c r="FO9" s="25"/>
+      <c r="FP9" s="25"/>
+      <c r="FQ9" s="25"/>
+      <c r="FR9" s="25"/>
+      <c r="FS9" s="25"/>
+      <c r="FT9" s="25"/>
+      <c r="FU9" s="25"/>
+      <c r="FV9" s="25"/>
+      <c r="FW9" s="25"/>
+      <c r="FX9" s="25"/>
+      <c r="FY9" s="25"/>
+      <c r="FZ9" s="25"/>
+      <c r="GA9" s="25"/>
+      <c r="GB9" s="25"/>
+      <c r="GC9" s="25"/>
+      <c r="GD9" s="25"/>
+      <c r="GE9" s="25"/>
+      <c r="GF9" s="25"/>
+      <c r="GG9" s="25"/>
+      <c r="GH9" s="25"/>
+      <c r="GI9" s="25"/>
+      <c r="GJ9" s="25"/>
+      <c r="GK9" s="25"/>
+      <c r="GL9" s="25"/>
+      <c r="GM9" s="25"/>
+      <c r="GN9" s="25"/>
+      <c r="GO9" s="25"/>
+      <c r="GP9" s="25"/>
+      <c r="GQ9" s="25"/>
+      <c r="GR9" s="25"/>
+      <c r="GS9" s="25"/>
+      <c r="GT9" s="25"/>
+      <c r="GU9" s="25"/>
+      <c r="GV9" s="25"/>
+      <c r="GW9" s="25"/>
+      <c r="GX9" s="25"/>
+      <c r="GY9" s="25"/>
+      <c r="GZ9" s="25"/>
+      <c r="HA9" s="25"/>
+      <c r="HB9" s="25"/>
+      <c r="HC9" s="25"/>
+      <c r="HD9" s="25"/>
+      <c r="HE9" s="25"/>
+      <c r="HF9" s="25"/>
+      <c r="HG9" s="25"/>
+      <c r="HH9" s="25"/>
+      <c r="HI9" s="25"/>
+      <c r="HJ9" s="25"/>
+      <c r="HK9" s="25"/>
+      <c r="HL9" s="25"/>
+      <c r="HM9" s="25"/>
+      <c r="HN9" s="25"/>
+      <c r="HO9" s="25"/>
+      <c r="HP9" s="25"/>
+      <c r="HQ9" s="25"/>
+      <c r="HR9" s="25"/>
+      <c r="HS9" s="25"/>
+      <c r="HT9" s="25"/>
+      <c r="HU9" s="25"/>
+      <c r="HV9" s="25"/>
+      <c r="HW9" s="25"/>
+      <c r="HX9" s="25"/>
+      <c r="HY9" s="25"/>
+      <c r="HZ9" s="25"/>
+      <c r="IA9" s="25"/>
+      <c r="IB9" s="25"/>
+      <c r="IC9" s="25"/>
+      <c r="ID9" s="25"/>
+      <c r="IE9" s="25"/>
+      <c r="IF9" s="25"/>
+      <c r="IG9" s="25"/>
+      <c r="IH9" s="25"/>
+      <c r="II9" s="25"/>
+      <c r="IJ9" s="25"/>
+      <c r="IK9" s="25"/>
+      <c r="IL9" s="25"/>
+      <c r="IM9" s="25"/>
+      <c r="IN9" s="25"/>
+      <c r="IO9" s="25"/>
+      <c r="IP9" s="25"/>
+      <c r="IQ9" s="25"/>
+      <c r="IR9" s="25"/>
+      <c r="IS9" s="25"/>
+      <c r="IT9" s="25"/>
+      <c r="IU9" s="25"/>
+      <c r="IV9" s="25"/>
+      <c r="IW9" s="25"/>
+      <c r="IX9" s="25"/>
+      <c r="IY9" s="25"/>
+      <c r="IZ9" s="25"/>
+      <c r="JA9" s="25"/>
+      <c r="JB9" s="25"/>
+      <c r="JC9" s="25"/>
+      <c r="JD9" s="25"/>
+      <c r="JE9" s="25"/>
+      <c r="JF9" s="25"/>
+      <c r="JG9" s="25"/>
+      <c r="JH9" s="25"/>
+      <c r="JI9" s="25"/>
+      <c r="JJ9" s="25"/>
+      <c r="JK9" s="25"/>
+      <c r="JL9" s="25"/>
+      <c r="JM9" s="25"/>
+      <c r="JN9" s="25"/>
+      <c r="JO9" s="25"/>
+      <c r="JP9" s="25"/>
+      <c r="JQ9" s="25"/>
+      <c r="JR9" s="25"/>
+      <c r="JS9" s="25"/>
+      <c r="JT9" s="25"/>
+      <c r="JU9" s="25"/>
+      <c r="JV9" s="25"/>
+      <c r="JW9" s="25"/>
+      <c r="JX9" s="25"/>
+      <c r="JY9" s="25"/>
+      <c r="JZ9" s="25"/>
+      <c r="KA9" s="25"/>
+      <c r="KB9" s="25"/>
+      <c r="KC9" s="25"/>
+      <c r="KD9" s="25"/>
+      <c r="KE9" s="25"/>
+      <c r="KF9" s="25"/>
+      <c r="KG9" s="25"/>
+      <c r="KH9" s="25"/>
+      <c r="KI9" s="25"/>
+      <c r="KJ9" s="25"/>
+      <c r="KK9" s="25"/>
+      <c r="KL9" s="25"/>
+      <c r="KM9" s="25"/>
+      <c r="KN9" s="25"/>
+      <c r="KO9" s="25"/>
+      <c r="KP9" s="25"/>
+      <c r="KQ9" s="25"/>
+      <c r="KR9" s="25"/>
+      <c r="KS9" s="25"/>
+      <c r="KT9" s="25"/>
+      <c r="KU9" s="25"/>
+      <c r="KV9" s="25"/>
+      <c r="KW9" s="25"/>
+      <c r="KX9" s="25"/>
+      <c r="KY9" s="25"/>
+      <c r="KZ9" s="25"/>
+      <c r="LA9" s="25"/>
+      <c r="LB9" s="25"/>
+      <c r="LC9" s="25"/>
+      <c r="LD9" s="25"/>
+      <c r="LE9" s="25"/>
+      <c r="LF9" s="25"/>
+      <c r="LG9" s="25"/>
+      <c r="LH9" s="25"/>
+      <c r="LI9" s="25"/>
+      <c r="LJ9" s="25"/>
+      <c r="LK9" s="25"/>
+      <c r="LL9" s="25"/>
+      <c r="LM9" s="25"/>
+      <c r="LN9" s="25"/>
+      <c r="LO9" s="25"/>
+      <c r="LP9" s="25"/>
+      <c r="LQ9" s="25"/>
+      <c r="LR9" s="25"/>
+      <c r="LS9" s="25"/>
+      <c r="LT9" s="25"/>
+      <c r="LU9" s="25"/>
+      <c r="LV9" s="25"/>
+      <c r="LW9" s="25"/>
+      <c r="LX9" s="25"/>
+      <c r="LY9" s="25"/>
+      <c r="LZ9" s="25"/>
+      <c r="MA9" s="25"/>
+      <c r="MB9" s="25"/>
+      <c r="MC9" s="25"/>
+      <c r="MD9" s="25"/>
+      <c r="ME9" s="25"/>
+      <c r="MF9" s="25"/>
+      <c r="MG9" s="25"/>
+      <c r="MH9" s="25"/>
+      <c r="MI9" s="25"/>
+      <c r="MJ9" s="25"/>
+      <c r="MK9" s="25"/>
+      <c r="ML9" s="25"/>
+      <c r="MM9" s="25"/>
+      <c r="MN9" s="25"/>
+      <c r="MO9" s="25"/>
+      <c r="MP9" s="25"/>
+      <c r="MQ9" s="25"/>
+      <c r="MR9" s="25"/>
+      <c r="MS9" s="25"/>
+      <c r="MT9" s="25"/>
+      <c r="MU9" s="25"/>
+      <c r="MV9" s="25"/>
+      <c r="MW9" s="25"/>
+      <c r="MX9" s="25"/>
+      <c r="MY9" s="25"/>
+      <c r="MZ9" s="25"/>
+      <c r="NA9" s="25"/>
+      <c r="NB9" s="25"/>
+      <c r="NC9" s="25"/>
+      <c r="ND9" s="25"/>
+      <c r="NE9" s="25"/>
+      <c r="NF9" s="25"/>
+      <c r="NG9" s="25"/>
+      <c r="NH9" s="25"/>
+      <c r="NI9" s="25"/>
+      <c r="NJ9" s="25"/>
+      <c r="NK9" s="25"/>
+      <c r="NL9" s="25"/>
+      <c r="NM9" s="25"/>
+      <c r="NN9" s="25"/>
+      <c r="NO9" s="25"/>
+      <c r="NP9" s="25"/>
+      <c r="NQ9" s="25"/>
+      <c r="NR9" s="25"/>
+      <c r="NS9" s="25"/>
+      <c r="NT9" s="25"/>
+      <c r="NU9" s="25"/>
+      <c r="NV9" s="25"/>
+      <c r="NW9" s="25"/>
+      <c r="NX9" s="25"/>
+      <c r="NY9" s="25"/>
+      <c r="NZ9" s="25"/>
+      <c r="OA9" s="25"/>
+      <c r="OB9" s="25"/>
+      <c r="OC9" s="25"/>
+      <c r="OD9" s="25"/>
+      <c r="OE9" s="25"/>
+      <c r="OF9" s="25"/>
+      <c r="OG9" s="25"/>
+      <c r="OH9" s="25"/>
+      <c r="OI9" s="25"/>
+      <c r="OJ9" s="25"/>
+      <c r="OK9" s="25"/>
+      <c r="OL9" s="25"/>
+      <c r="OM9" s="25"/>
+      <c r="ON9" s="25"/>
+      <c r="OO9" s="25"/>
+      <c r="OP9" s="25"/>
+      <c r="OQ9" s="25"/>
+      <c r="OR9" s="25"/>
+      <c r="OS9" s="25"/>
+      <c r="OT9" s="25"/>
+      <c r="OU9" s="25"/>
+      <c r="OV9" s="25"/>
+      <c r="OW9" s="25"/>
+      <c r="OX9" s="25"/>
+      <c r="OY9" s="25"/>
+      <c r="OZ9" s="25"/>
+      <c r="PA9" s="25"/>
+      <c r="PB9" s="25"/>
+      <c r="PC9" s="25"/>
+      <c r="PD9" s="25"/>
+      <c r="PE9" s="25"/>
+      <c r="PF9" s="25"/>
+      <c r="PG9" s="25"/>
+      <c r="PH9" s="25"/>
+      <c r="PI9" s="25"/>
+      <c r="PJ9" s="25"/>
+      <c r="PK9" s="25"/>
+      <c r="PL9" s="25"/>
+      <c r="PM9" s="25"/>
+      <c r="PN9" s="25"/>
+      <c r="PO9" s="25"/>
+      <c r="PP9" s="25"/>
+      <c r="PQ9" s="25"/>
+      <c r="PR9" s="25"/>
+      <c r="PS9" s="25"/>
+      <c r="PT9" s="25"/>
+      <c r="PU9" s="25"/>
+      <c r="PV9" s="25"/>
+      <c r="PW9" s="25"/>
+      <c r="PX9" s="25"/>
+      <c r="PY9" s="25"/>
+      <c r="PZ9" s="25"/>
+      <c r="QA9" s="25"/>
+      <c r="QB9" s="25"/>
+      <c r="QC9" s="25"/>
+      <c r="QD9" s="25"/>
+      <c r="QE9" s="25"/>
+      <c r="QF9" s="25"/>
+      <c r="QG9" s="25"/>
+      <c r="QH9" s="25"/>
+      <c r="QI9" s="25"/>
+      <c r="QJ9" s="25"/>
+      <c r="QK9" s="25"/>
+      <c r="QL9" s="25"/>
+      <c r="QM9" s="25"/>
+      <c r="QN9" s="25"/>
+      <c r="QO9" s="25"/>
+      <c r="QP9" s="25"/>
+      <c r="QQ9" s="25"/>
+      <c r="QR9" s="25"/>
+      <c r="QS9" s="25"/>
+      <c r="QT9" s="25"/>
+      <c r="QU9" s="25"/>
+      <c r="QV9" s="25"/>
+      <c r="QW9" s="25"/>
+      <c r="QX9" s="25"/>
+      <c r="QY9" s="25"/>
+      <c r="QZ9" s="25"/>
+      <c r="RA9" s="25"/>
+      <c r="RB9" s="25"/>
+      <c r="RC9" s="25"/>
+      <c r="RD9" s="25"/>
+      <c r="RE9" s="25"/>
+      <c r="RF9" s="25"/>
+      <c r="RG9" s="25"/>
+      <c r="RH9" s="25"/>
+      <c r="RI9" s="25"/>
+      <c r="RJ9" s="25"/>
+      <c r="RK9" s="25"/>
+      <c r="RL9" s="25"/>
+      <c r="RM9" s="25"/>
+      <c r="RN9" s="25"/>
+      <c r="RO9" s="25"/>
+      <c r="RP9" s="25"/>
+      <c r="RQ9" s="25"/>
+      <c r="RR9" s="25"/>
+      <c r="RS9" s="25"/>
+      <c r="RT9" s="25"/>
+      <c r="RU9" s="25"/>
+      <c r="RV9" s="25"/>
+      <c r="RW9" s="25"/>
+      <c r="RX9" s="25"/>
+      <c r="RY9" s="25"/>
+      <c r="RZ9" s="25"/>
+      <c r="SA9" s="25"/>
+      <c r="SB9" s="25"/>
+      <c r="SC9" s="25"/>
+      <c r="SD9" s="25"/>
+      <c r="SE9" s="25"/>
+      <c r="SF9" s="25"/>
+      <c r="SG9" s="25"/>
+      <c r="SH9" s="25"/>
+      <c r="SI9" s="25"/>
+      <c r="SJ9" s="25"/>
+      <c r="SK9" s="25"/>
+      <c r="SL9" s="25"/>
+      <c r="SM9" s="25"/>
+      <c r="SN9" s="25"/>
+      <c r="SO9" s="25"/>
+      <c r="SP9" s="25"/>
+      <c r="SQ9" s="25"/>
+      <c r="SR9" s="25"/>
+      <c r="SS9" s="25"/>
+      <c r="ST9" s="25"/>
+      <c r="SU9" s="25"/>
+      <c r="SV9" s="25"/>
+      <c r="SW9" s="25"/>
+      <c r="SX9" s="25"/>
+      <c r="SY9" s="25"/>
+      <c r="SZ9" s="25"/>
+      <c r="TA9" s="25"/>
+      <c r="TB9" s="25"/>
+      <c r="TC9" s="25"/>
+      <c r="TD9" s="25"/>
+      <c r="TE9" s="25"/>
+      <c r="TF9" s="25"/>
+      <c r="TG9" s="25"/>
+      <c r="TH9" s="25"/>
+      <c r="TI9" s="25"/>
+      <c r="TJ9" s="25"/>
+      <c r="TK9" s="25"/>
+      <c r="TL9" s="25"/>
+      <c r="TM9" s="25"/>
+      <c r="TN9" s="25"/>
+      <c r="TO9" s="25"/>
+      <c r="TP9" s="25"/>
+      <c r="TQ9" s="25"/>
+      <c r="TR9" s="25"/>
+      <c r="TS9" s="25"/>
+      <c r="TT9" s="25"/>
+      <c r="TU9" s="25"/>
+      <c r="TV9" s="25"/>
+      <c r="TW9" s="25"/>
+      <c r="TX9" s="25"/>
+      <c r="TY9" s="25"/>
+      <c r="TZ9" s="25"/>
+      <c r="UA9" s="25"/>
+      <c r="UB9" s="25"/>
+      <c r="UC9" s="25"/>
+      <c r="UD9" s="25"/>
+      <c r="UE9" s="25"/>
+      <c r="UF9" s="25"/>
+      <c r="UG9" s="25"/>
+      <c r="UH9" s="25"/>
+      <c r="UI9" s="25"/>
+      <c r="UJ9" s="25"/>
+      <c r="UK9" s="25"/>
+      <c r="UL9" s="25"/>
+      <c r="UM9" s="25"/>
+      <c r="UN9" s="25"/>
+      <c r="UO9" s="25"/>
+      <c r="UP9" s="25"/>
+      <c r="UQ9" s="25"/>
+      <c r="UR9" s="25"/>
+      <c r="US9" s="25"/>
+      <c r="UT9" s="25"/>
+      <c r="UU9" s="25"/>
+      <c r="UV9" s="25"/>
+      <c r="UW9" s="25"/>
+      <c r="UX9" s="25"/>
+      <c r="UY9" s="25"/>
+      <c r="UZ9" s="25"/>
+      <c r="VA9" s="25"/>
+      <c r="VB9" s="25"/>
+      <c r="VC9" s="25"/>
+      <c r="VD9" s="25"/>
+      <c r="VE9" s="25"/>
+      <c r="VF9" s="25"/>
+      <c r="VG9" s="25"/>
+      <c r="VH9" s="25"/>
+      <c r="VI9" s="25"/>
+      <c r="VJ9" s="25"/>
+      <c r="VK9" s="25"/>
+      <c r="VL9" s="25"/>
+      <c r="VM9" s="25"/>
+      <c r="VN9" s="25"/>
+      <c r="VO9" s="25"/>
+      <c r="VP9" s="25"/>
+      <c r="VQ9" s="25"/>
+      <c r="VR9" s="25"/>
+      <c r="VS9" s="25"/>
+      <c r="VT9" s="25"/>
+      <c r="VU9" s="25"/>
+      <c r="VV9" s="25"/>
+      <c r="VW9" s="25"/>
+      <c r="VX9" s="25"/>
+      <c r="VY9" s="25"/>
+      <c r="VZ9" s="25"/>
+      <c r="WA9" s="25"/>
+      <c r="WB9" s="25"/>
+      <c r="WC9" s="25"/>
+      <c r="WD9" s="25"/>
+      <c r="WE9" s="25"/>
+      <c r="WF9" s="25"/>
+      <c r="WG9" s="25"/>
+      <c r="WH9" s="25"/>
+      <c r="WI9" s="25"/>
+      <c r="WJ9" s="25"/>
+      <c r="WK9" s="25"/>
+      <c r="WL9" s="25"/>
+      <c r="WM9" s="25"/>
+      <c r="WN9" s="25"/>
+      <c r="WO9" s="25"/>
+      <c r="WP9" s="25"/>
+      <c r="WQ9" s="25"/>
+      <c r="WR9" s="25"/>
+      <c r="WS9" s="25"/>
+      <c r="WT9" s="25"/>
+      <c r="WU9" s="25"/>
+      <c r="WV9" s="25"/>
+      <c r="WW9" s="25"/>
+      <c r="WX9" s="25"/>
+      <c r="WY9" s="25"/>
+      <c r="WZ9" s="25"/>
+      <c r="XA9" s="25"/>
+      <c r="XB9" s="25"/>
+      <c r="XC9" s="25"/>
+      <c r="XD9" s="25"/>
+      <c r="XE9" s="25"/>
+      <c r="XF9" s="25"/>
+      <c r="XG9" s="25"/>
+      <c r="XH9" s="25"/>
+      <c r="XI9" s="25"/>
+      <c r="XJ9" s="25"/>
+      <c r="XK9" s="25"/>
+      <c r="XL9" s="25"/>
+      <c r="XM9" s="25"/>
+      <c r="XN9" s="25"/>
+      <c r="XO9" s="25"/>
+      <c r="XP9" s="25"/>
+      <c r="XQ9" s="25"/>
+      <c r="XR9" s="25"/>
+      <c r="XS9" s="25"/>
+      <c r="XT9" s="25"/>
+      <c r="XU9" s="25"/>
+      <c r="XV9" s="25"/>
+      <c r="XW9" s="25"/>
+      <c r="XX9" s="25"/>
+      <c r="XY9" s="25"/>
+      <c r="XZ9" s="25"/>
+      <c r="YA9" s="25"/>
+      <c r="YB9" s="25"/>
+      <c r="YC9" s="25"/>
+      <c r="YD9" s="25"/>
+      <c r="YE9" s="25"/>
+      <c r="YF9" s="25"/>
+      <c r="YG9" s="25"/>
+      <c r="YH9" s="25"/>
+      <c r="YI9" s="25"/>
+      <c r="YJ9" s="25"/>
+      <c r="YK9" s="25"/>
+      <c r="YL9" s="25"/>
+      <c r="YM9" s="25"/>
+      <c r="YN9" s="25"/>
+      <c r="YO9" s="25"/>
+      <c r="YP9" s="25"/>
+      <c r="YQ9" s="25"/>
+      <c r="YR9" s="25"/>
+      <c r="YS9" s="25"/>
+      <c r="YT9" s="25"/>
+      <c r="YU9" s="25"/>
+      <c r="YV9" s="25"/>
+      <c r="YW9" s="25"/>
+      <c r="YX9" s="25"/>
+      <c r="YY9" s="25"/>
+      <c r="YZ9" s="25"/>
+      <c r="ZA9" s="25"/>
+      <c r="ZB9" s="25"/>
+      <c r="ZC9" s="25"/>
+      <c r="ZD9" s="25"/>
+      <c r="ZE9" s="25"/>
+      <c r="ZF9" s="25"/>
+      <c r="ZG9" s="25"/>
+      <c r="ZH9" s="25"/>
+      <c r="ZI9" s="25"/>
+      <c r="ZJ9" s="25"/>
+      <c r="ZK9" s="25"/>
+      <c r="ZL9" s="25"/>
+      <c r="ZM9" s="25"/>
+      <c r="ZN9" s="25"/>
+      <c r="ZO9" s="25"/>
+      <c r="ZP9" s="25"/>
+      <c r="ZQ9" s="25"/>
+      <c r="ZR9" s="25"/>
+      <c r="ZS9" s="25"/>
+      <c r="ZT9" s="25"/>
+      <c r="ZU9" s="25"/>
+      <c r="ZV9" s="25"/>
+      <c r="ZW9" s="25"/>
+      <c r="ZX9" s="25"/>
+      <c r="ZY9" s="25"/>
+      <c r="ZZ9" s="25"/>
+      <c r="AAA9" s="25"/>
+      <c r="AAB9" s="25"/>
+      <c r="AAC9" s="25"/>
+      <c r="AAD9" s="25"/>
+      <c r="AAE9" s="25"/>
+      <c r="AAF9" s="25"/>
+      <c r="AAG9" s="25"/>
+      <c r="AAH9" s="25"/>
+      <c r="AAI9" s="25"/>
+      <c r="AAJ9" s="25"/>
+      <c r="AAK9" s="25"/>
+      <c r="AAL9" s="25"/>
+      <c r="AAM9" s="25"/>
+      <c r="AAN9" s="25"/>
+      <c r="AAO9" s="25"/>
+      <c r="AAP9" s="25"/>
+      <c r="AAQ9" s="25"/>
+      <c r="AAR9" s="25"/>
+      <c r="AAS9" s="25"/>
+      <c r="AAT9" s="25"/>
+      <c r="AAU9" s="25"/>
+      <c r="AAV9" s="25"/>
+      <c r="AAW9" s="25"/>
+      <c r="AAX9" s="25"/>
+      <c r="AAY9" s="25"/>
+      <c r="AAZ9" s="25"/>
+      <c r="ABA9" s="25"/>
+      <c r="ABB9" s="25"/>
+      <c r="ABC9" s="25"/>
+      <c r="ABD9" s="25"/>
+      <c r="ABE9" s="25"/>
+      <c r="ABF9" s="25"/>
+      <c r="ABG9" s="25"/>
+      <c r="ABH9" s="25"/>
+      <c r="ABI9" s="25"/>
+      <c r="ABJ9" s="25"/>
+      <c r="ABK9" s="25"/>
+      <c r="ABL9" s="25"/>
+      <c r="ABM9" s="25"/>
+      <c r="ABN9" s="25"/>
+      <c r="ABO9" s="25"/>
+      <c r="ABP9" s="25"/>
+      <c r="ABQ9" s="25"/>
+      <c r="ABR9" s="25"/>
+      <c r="ABS9" s="25"/>
+      <c r="ABT9" s="25"/>
+      <c r="ABU9" s="25"/>
+      <c r="ABV9" s="25"/>
+      <c r="ABW9" s="25"/>
+      <c r="ABX9" s="25"/>
+      <c r="ABY9" s="25"/>
+      <c r="ABZ9" s="25"/>
+      <c r="ACA9" s="25"/>
+      <c r="ACB9" s="25"/>
+      <c r="ACC9" s="25"/>
+      <c r="ACD9" s="25"/>
+      <c r="ACE9" s="25"/>
+      <c r="ACF9" s="25"/>
+      <c r="ACG9" s="25"/>
+      <c r="ACH9" s="25"/>
+      <c r="ACI9" s="25"/>
+      <c r="ACJ9" s="25"/>
+      <c r="ACK9" s="25"/>
+      <c r="ACL9" s="25"/>
+      <c r="ACM9" s="25"/>
+      <c r="ACN9" s="25"/>
+      <c r="ACO9" s="25"/>
+      <c r="ACP9" s="25"/>
+      <c r="ACQ9" s="25"/>
+      <c r="ACR9" s="25"/>
+      <c r="ACS9" s="25"/>
+      <c r="ACT9" s="25"/>
+      <c r="ACU9" s="25"/>
+      <c r="ACV9" s="25"/>
+      <c r="ACW9" s="25"/>
+      <c r="ACX9" s="25"/>
+      <c r="ACY9" s="25"/>
+      <c r="ACZ9" s="25"/>
+      <c r="ADA9" s="25"/>
+      <c r="ADB9" s="25"/>
+      <c r="ADC9" s="25"/>
+      <c r="ADD9" s="25"/>
+      <c r="ADE9" s="25"/>
+      <c r="ADF9" s="25"/>
+      <c r="ADG9" s="25"/>
+      <c r="ADH9" s="25"/>
+      <c r="ADI9" s="25"/>
+      <c r="ADJ9" s="25"/>
+      <c r="ADK9" s="25"/>
+      <c r="ADL9" s="25"/>
+      <c r="ADM9" s="25"/>
+      <c r="ADN9" s="25"/>
+      <c r="ADO9" s="25"/>
+      <c r="ADP9" s="25"/>
+      <c r="ADQ9" s="25"/>
+      <c r="ADR9" s="25"/>
+      <c r="ADS9" s="25"/>
+      <c r="ADT9" s="25"/>
+      <c r="ADU9" s="25"/>
+      <c r="ADV9" s="25"/>
+      <c r="ADW9" s="25"/>
+      <c r="ADX9" s="25"/>
+      <c r="ADY9" s="25"/>
+      <c r="ADZ9" s="25"/>
+      <c r="AEA9" s="25"/>
+      <c r="AEB9" s="25"/>
+      <c r="AEC9" s="25"/>
+      <c r="AED9" s="25"/>
+      <c r="AEE9" s="25"/>
+      <c r="AEF9" s="25"/>
+      <c r="AEG9" s="25"/>
+      <c r="AEH9" s="25"/>
+      <c r="AEI9" s="25"/>
+      <c r="AEJ9" s="25"/>
+      <c r="AEK9" s="25"/>
+      <c r="AEL9" s="25"/>
+      <c r="AEM9" s="25"/>
+      <c r="AEN9" s="25"/>
+      <c r="AEO9" s="25"/>
+      <c r="AEP9" s="25"/>
+      <c r="AEQ9" s="25"/>
+      <c r="AER9" s="25"/>
+      <c r="AES9" s="25"/>
+      <c r="AET9" s="25"/>
+      <c r="AEU9" s="25"/>
+      <c r="AEV9" s="25"/>
+      <c r="AEW9" s="25"/>
+      <c r="AEX9" s="25"/>
+      <c r="AEY9" s="25"/>
+      <c r="AEZ9" s="25"/>
+      <c r="AFA9" s="25"/>
+      <c r="AFB9" s="25"/>
+      <c r="AFC9" s="25"/>
+      <c r="AFD9" s="25"/>
+      <c r="AFE9" s="25"/>
+      <c r="AFF9" s="25"/>
+      <c r="AFG9" s="25"/>
+      <c r="AFH9" s="25"/>
+      <c r="AFI9" s="25"/>
+      <c r="AFJ9" s="25"/>
+      <c r="AFK9" s="25"/>
+      <c r="AFL9" s="25"/>
+      <c r="AFM9" s="25"/>
+      <c r="AFN9" s="25"/>
+      <c r="AFO9" s="25"/>
+      <c r="AFP9" s="25"/>
+      <c r="AFQ9" s="25"/>
+      <c r="AFR9" s="25"/>
+      <c r="AFS9" s="25"/>
+      <c r="AFT9" s="25"/>
+      <c r="AFU9" s="25"/>
+      <c r="AFV9" s="25"/>
+      <c r="AFW9" s="25"/>
+      <c r="AFX9" s="25"/>
+      <c r="AFY9" s="25"/>
+      <c r="AFZ9" s="25"/>
+      <c r="AGA9" s="25"/>
+      <c r="AGB9" s="25"/>
+      <c r="AGC9" s="25"/>
+      <c r="AGD9" s="25"/>
+      <c r="AGE9" s="25"/>
+      <c r="AGF9" s="25"/>
+      <c r="AGG9" s="25"/>
+      <c r="AGH9" s="25"/>
+      <c r="AGI9" s="25"/>
+      <c r="AGJ9" s="25"/>
+      <c r="AGK9" s="25"/>
+      <c r="AGL9" s="25"/>
+      <c r="AGM9" s="25"/>
+      <c r="AGN9" s="25"/>
+      <c r="AGO9" s="25"/>
+      <c r="AGP9" s="25"/>
+      <c r="AGQ9" s="25"/>
+      <c r="AGR9" s="25"/>
+      <c r="AGS9" s="25"/>
+      <c r="AGT9" s="25"/>
+      <c r="AGU9" s="25"/>
+      <c r="AGV9" s="25"/>
+      <c r="AGW9" s="25"/>
+      <c r="AGX9" s="25"/>
+      <c r="AGY9" s="25"/>
+      <c r="AGZ9" s="25"/>
+      <c r="AHA9" s="25"/>
+      <c r="AHB9" s="25"/>
+      <c r="AHC9" s="25"/>
+      <c r="AHD9" s="25"/>
+      <c r="AHE9" s="25"/>
+      <c r="AHF9" s="25"/>
+      <c r="AHG9" s="25"/>
+      <c r="AHH9" s="25"/>
+      <c r="AHI9" s="25"/>
+      <c r="AHJ9" s="25"/>
+      <c r="AHK9" s="25"/>
+      <c r="AHL9" s="25"/>
+      <c r="AHM9" s="25"/>
+      <c r="AHN9" s="25"/>
+      <c r="AHO9" s="25"/>
+      <c r="AHP9" s="25"/>
+      <c r="AHQ9" s="25"/>
+      <c r="AHR9" s="25"/>
+      <c r="AHS9" s="25"/>
+      <c r="AHT9" s="25"/>
+      <c r="AHU9" s="25"/>
+      <c r="AHV9" s="25"/>
+      <c r="AHW9" s="25"/>
+      <c r="AHX9" s="25"/>
+      <c r="AHY9" s="25"/>
+      <c r="AHZ9" s="25"/>
+      <c r="AIA9" s="25"/>
+      <c r="AIB9" s="25"/>
+      <c r="AIC9" s="25"/>
+      <c r="AID9" s="25"/>
+      <c r="AIE9" s="25"/>
+      <c r="AIF9" s="25"/>
+      <c r="AIG9" s="25"/>
+      <c r="AIH9" s="25"/>
+      <c r="AII9" s="25"/>
+      <c r="AIJ9" s="25"/>
+      <c r="AIK9" s="25"/>
+      <c r="AIL9" s="25"/>
+      <c r="AIM9" s="25"/>
+      <c r="AIN9" s="25"/>
+      <c r="AIO9" s="25"/>
+      <c r="AIP9" s="25"/>
+      <c r="AIQ9" s="25"/>
+      <c r="AIR9" s="25"/>
+      <c r="AIS9" s="25"/>
+      <c r="AIT9" s="25"/>
+      <c r="AIU9" s="25"/>
+      <c r="AIV9" s="25"/>
+      <c r="AIW9" s="25"/>
+      <c r="AIX9" s="25"/>
+      <c r="AIY9" s="25"/>
+      <c r="AIZ9" s="25"/>
+      <c r="AJA9" s="25"/>
+      <c r="AJB9" s="25"/>
+      <c r="AJC9" s="25"/>
+      <c r="AJD9" s="25"/>
+      <c r="AJE9" s="25"/>
+      <c r="AJF9" s="25"/>
+      <c r="AJG9" s="25"/>
+      <c r="AJH9" s="25"/>
+      <c r="AJI9" s="25"/>
+      <c r="AJJ9" s="25"/>
+      <c r="AJK9" s="25"/>
+      <c r="AJL9" s="25"/>
+      <c r="AJM9" s="25"/>
+      <c r="AJN9" s="25"/>
+      <c r="AJO9" s="25"/>
+      <c r="AJP9" s="25"/>
+      <c r="AJQ9" s="25"/>
+      <c r="AJR9" s="25"/>
+      <c r="AJS9" s="25"/>
+      <c r="AJT9" s="25"/>
+      <c r="AJU9" s="25"/>
+      <c r="AJV9" s="25"/>
+      <c r="AJW9" s="25"/>
+      <c r="AJX9" s="25"/>
+      <c r="AJY9" s="25"/>
+      <c r="AJZ9" s="25"/>
+      <c r="AKA9" s="25"/>
+      <c r="AKB9" s="25"/>
+      <c r="AKC9" s="25"/>
+      <c r="AKD9" s="25"/>
+      <c r="AKE9" s="25"/>
+      <c r="AKF9" s="25"/>
+      <c r="AKG9" s="25"/>
+      <c r="AKH9" s="25"/>
+      <c r="AKI9" s="25"/>
+      <c r="AKJ9" s="25"/>
+      <c r="AKK9" s="25"/>
+      <c r="AKL9" s="25"/>
+      <c r="AKM9" s="25"/>
+      <c r="AKN9" s="25"/>
+      <c r="AKO9" s="25"/>
+      <c r="AKP9" s="25"/>
+      <c r="AKQ9" s="25"/>
+      <c r="AKR9" s="25"/>
+      <c r="AKS9" s="25"/>
+      <c r="AKT9" s="25"/>
+      <c r="AKU9" s="25"/>
+      <c r="AKV9" s="25"/>
+      <c r="AKW9" s="25"/>
+      <c r="AKX9" s="25"/>
+      <c r="AKY9" s="25"/>
+      <c r="AKZ9" s="25"/>
+      <c r="ALA9" s="25"/>
+      <c r="ALB9" s="25"/>
+      <c r="ALC9" s="25"/>
+      <c r="ALD9" s="25"/>
+      <c r="ALE9" s="25"/>
+      <c r="ALF9" s="25"/>
+      <c r="ALG9" s="25"/>
+      <c r="ALH9" s="25"/>
+      <c r="ALI9" s="25"/>
+      <c r="ALJ9" s="25"/>
+      <c r="ALK9" s="25"/>
+      <c r="ALL9" s="25"/>
+      <c r="ALM9" s="25"/>
+      <c r="ALN9" s="25"/>
+      <c r="ALO9" s="25"/>
+      <c r="ALP9" s="25"/>
+      <c r="ALQ9" s="25"/>
+      <c r="ALR9" s="25"/>
+      <c r="ALS9" s="25"/>
+      <c r="ALT9" s="25"/>
+      <c r="ALU9" s="25"/>
+      <c r="ALV9" s="25"/>
+      <c r="ALW9" s="25"/>
+      <c r="ALX9" s="25"/>
+      <c r="ALY9" s="25"/>
+      <c r="ALZ9" s="25"/>
+      <c r="AMA9" s="25"/>
+      <c r="AMB9" s="25"/>
+      <c r="AMC9" s="25"/>
+      <c r="AMD9" s="25"/>
+      <c r="AME9" s="25"/>
+      <c r="AMF9" s="25"/>
+      <c r="AMG9" s="25"/>
+      <c r="AMH9" s="25"/>
+      <c r="AMI9" s="25"/>
+      <c r="AMJ9" s="25"/>
+    </row>
+    <row r="10" spans="1:1024" s="32" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="5">
+      <c r="F10" s="34"/>
+      <c r="G10" s="29">
         <v>42286</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="30">
         <v>0</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="35" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="25"/>
+      <c r="AE10" s="25"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="25"/>
+      <c r="AI10" s="25"/>
+      <c r="AJ10" s="25"/>
+      <c r="AK10" s="25"/>
+      <c r="AL10" s="25"/>
+      <c r="AM10" s="25"/>
+      <c r="AN10" s="25"/>
+      <c r="AO10" s="25"/>
+      <c r="AP10" s="25"/>
+      <c r="AQ10" s="25"/>
+      <c r="AR10" s="25"/>
+      <c r="AS10" s="25"/>
+      <c r="AT10" s="25"/>
+      <c r="AU10" s="25"/>
+      <c r="AV10" s="25"/>
+      <c r="AW10" s="25"/>
+      <c r="AX10" s="25"/>
+      <c r="AY10" s="25"/>
+      <c r="AZ10" s="25"/>
+      <c r="BA10" s="25"/>
+      <c r="BB10" s="25"/>
+      <c r="BC10" s="25"/>
+      <c r="BD10" s="25"/>
+      <c r="BE10" s="25"/>
+      <c r="BF10" s="25"/>
+      <c r="BG10" s="25"/>
+      <c r="BH10" s="25"/>
+      <c r="BI10" s="25"/>
+      <c r="BJ10" s="25"/>
+      <c r="BK10" s="25"/>
+      <c r="BL10" s="25"/>
+      <c r="BM10" s="25"/>
+      <c r="BN10" s="25"/>
+      <c r="BO10" s="25"/>
+      <c r="BP10" s="25"/>
+      <c r="BQ10" s="25"/>
+      <c r="BR10" s="25"/>
+      <c r="BS10" s="25"/>
+      <c r="BT10" s="25"/>
+      <c r="BU10" s="25"/>
+      <c r="BV10" s="25"/>
+      <c r="BW10" s="25"/>
+      <c r="BX10" s="25"/>
+      <c r="BY10" s="25"/>
+      <c r="BZ10" s="25"/>
+      <c r="CA10" s="25"/>
+      <c r="CB10" s="25"/>
+      <c r="CC10" s="25"/>
+      <c r="CD10" s="25"/>
+      <c r="CE10" s="25"/>
+      <c r="CF10" s="25"/>
+      <c r="CG10" s="25"/>
+      <c r="CH10" s="25"/>
+      <c r="CI10" s="25"/>
+      <c r="CJ10" s="25"/>
+      <c r="CK10" s="25"/>
+      <c r="CL10" s="25"/>
+      <c r="CM10" s="25"/>
+      <c r="CN10" s="25"/>
+      <c r="CO10" s="25"/>
+      <c r="CP10" s="25"/>
+      <c r="CQ10" s="25"/>
+      <c r="CR10" s="25"/>
+      <c r="CS10" s="25"/>
+      <c r="CT10" s="25"/>
+      <c r="CU10" s="25"/>
+      <c r="CV10" s="25"/>
+      <c r="CW10" s="25"/>
+      <c r="CX10" s="25"/>
+      <c r="CY10" s="25"/>
+      <c r="CZ10" s="25"/>
+      <c r="DA10" s="25"/>
+      <c r="DB10" s="25"/>
+      <c r="DC10" s="25"/>
+      <c r="DD10" s="25"/>
+      <c r="DE10" s="25"/>
+      <c r="DF10" s="25"/>
+      <c r="DG10" s="25"/>
+      <c r="DH10" s="25"/>
+      <c r="DI10" s="25"/>
+      <c r="DJ10" s="25"/>
+      <c r="DK10" s="25"/>
+      <c r="DL10" s="25"/>
+      <c r="DM10" s="25"/>
+      <c r="DN10" s="25"/>
+      <c r="DO10" s="25"/>
+      <c r="DP10" s="25"/>
+      <c r="DQ10" s="25"/>
+      <c r="DR10" s="25"/>
+      <c r="DS10" s="25"/>
+      <c r="DT10" s="25"/>
+      <c r="DU10" s="25"/>
+      <c r="DV10" s="25"/>
+      <c r="DW10" s="25"/>
+      <c r="DX10" s="25"/>
+      <c r="DY10" s="25"/>
+      <c r="DZ10" s="25"/>
+      <c r="EA10" s="25"/>
+      <c r="EB10" s="25"/>
+      <c r="EC10" s="25"/>
+      <c r="ED10" s="25"/>
+      <c r="EE10" s="25"/>
+      <c r="EF10" s="25"/>
+      <c r="EG10" s="25"/>
+      <c r="EH10" s="25"/>
+      <c r="EI10" s="25"/>
+      <c r="EJ10" s="25"/>
+      <c r="EK10" s="25"/>
+      <c r="EL10" s="25"/>
+      <c r="EM10" s="25"/>
+      <c r="EN10" s="25"/>
+      <c r="EO10" s="25"/>
+      <c r="EP10" s="25"/>
+      <c r="EQ10" s="25"/>
+      <c r="ER10" s="25"/>
+      <c r="ES10" s="25"/>
+      <c r="ET10" s="25"/>
+      <c r="EU10" s="25"/>
+      <c r="EV10" s="25"/>
+      <c r="EW10" s="25"/>
+      <c r="EX10" s="25"/>
+      <c r="EY10" s="25"/>
+      <c r="EZ10" s="25"/>
+      <c r="FA10" s="25"/>
+      <c r="FB10" s="25"/>
+      <c r="FC10" s="25"/>
+      <c r="FD10" s="25"/>
+      <c r="FE10" s="25"/>
+      <c r="FF10" s="25"/>
+      <c r="FG10" s="25"/>
+      <c r="FH10" s="25"/>
+      <c r="FI10" s="25"/>
+      <c r="FJ10" s="25"/>
+      <c r="FK10" s="25"/>
+      <c r="FL10" s="25"/>
+      <c r="FM10" s="25"/>
+      <c r="FN10" s="25"/>
+      <c r="FO10" s="25"/>
+      <c r="FP10" s="25"/>
+      <c r="FQ10" s="25"/>
+      <c r="FR10" s="25"/>
+      <c r="FS10" s="25"/>
+      <c r="FT10" s="25"/>
+      <c r="FU10" s="25"/>
+      <c r="FV10" s="25"/>
+      <c r="FW10" s="25"/>
+      <c r="FX10" s="25"/>
+      <c r="FY10" s="25"/>
+      <c r="FZ10" s="25"/>
+      <c r="GA10" s="25"/>
+      <c r="GB10" s="25"/>
+      <c r="GC10" s="25"/>
+      <c r="GD10" s="25"/>
+      <c r="GE10" s="25"/>
+      <c r="GF10" s="25"/>
+      <c r="GG10" s="25"/>
+      <c r="GH10" s="25"/>
+      <c r="GI10" s="25"/>
+      <c r="GJ10" s="25"/>
+      <c r="GK10" s="25"/>
+      <c r="GL10" s="25"/>
+      <c r="GM10" s="25"/>
+      <c r="GN10" s="25"/>
+      <c r="GO10" s="25"/>
+      <c r="GP10" s="25"/>
+      <c r="GQ10" s="25"/>
+      <c r="GR10" s="25"/>
+      <c r="GS10" s="25"/>
+      <c r="GT10" s="25"/>
+      <c r="GU10" s="25"/>
+      <c r="GV10" s="25"/>
+      <c r="GW10" s="25"/>
+      <c r="GX10" s="25"/>
+      <c r="GY10" s="25"/>
+      <c r="GZ10" s="25"/>
+      <c r="HA10" s="25"/>
+      <c r="HB10" s="25"/>
+      <c r="HC10" s="25"/>
+      <c r="HD10" s="25"/>
+      <c r="HE10" s="25"/>
+      <c r="HF10" s="25"/>
+      <c r="HG10" s="25"/>
+      <c r="HH10" s="25"/>
+      <c r="HI10" s="25"/>
+      <c r="HJ10" s="25"/>
+      <c r="HK10" s="25"/>
+      <c r="HL10" s="25"/>
+      <c r="HM10" s="25"/>
+      <c r="HN10" s="25"/>
+      <c r="HO10" s="25"/>
+      <c r="HP10" s="25"/>
+      <c r="HQ10" s="25"/>
+      <c r="HR10" s="25"/>
+      <c r="HS10" s="25"/>
+      <c r="HT10" s="25"/>
+      <c r="HU10" s="25"/>
+      <c r="HV10" s="25"/>
+      <c r="HW10" s="25"/>
+      <c r="HX10" s="25"/>
+      <c r="HY10" s="25"/>
+      <c r="HZ10" s="25"/>
+      <c r="IA10" s="25"/>
+      <c r="IB10" s="25"/>
+      <c r="IC10" s="25"/>
+      <c r="ID10" s="25"/>
+      <c r="IE10" s="25"/>
+      <c r="IF10" s="25"/>
+      <c r="IG10" s="25"/>
+      <c r="IH10" s="25"/>
+      <c r="II10" s="25"/>
+      <c r="IJ10" s="25"/>
+      <c r="IK10" s="25"/>
+      <c r="IL10" s="25"/>
+      <c r="IM10" s="25"/>
+      <c r="IN10" s="25"/>
+      <c r="IO10" s="25"/>
+      <c r="IP10" s="25"/>
+      <c r="IQ10" s="25"/>
+      <c r="IR10" s="25"/>
+      <c r="IS10" s="25"/>
+      <c r="IT10" s="25"/>
+      <c r="IU10" s="25"/>
+      <c r="IV10" s="25"/>
+      <c r="IW10" s="25"/>
+      <c r="IX10" s="25"/>
+      <c r="IY10" s="25"/>
+      <c r="IZ10" s="25"/>
+      <c r="JA10" s="25"/>
+      <c r="JB10" s="25"/>
+      <c r="JC10" s="25"/>
+      <c r="JD10" s="25"/>
+      <c r="JE10" s="25"/>
+      <c r="JF10" s="25"/>
+      <c r="JG10" s="25"/>
+      <c r="JH10" s="25"/>
+      <c r="JI10" s="25"/>
+      <c r="JJ10" s="25"/>
+      <c r="JK10" s="25"/>
+      <c r="JL10" s="25"/>
+      <c r="JM10" s="25"/>
+      <c r="JN10" s="25"/>
+      <c r="JO10" s="25"/>
+      <c r="JP10" s="25"/>
+      <c r="JQ10" s="25"/>
+      <c r="JR10" s="25"/>
+      <c r="JS10" s="25"/>
+      <c r="JT10" s="25"/>
+      <c r="JU10" s="25"/>
+      <c r="JV10" s="25"/>
+      <c r="JW10" s="25"/>
+      <c r="JX10" s="25"/>
+      <c r="JY10" s="25"/>
+      <c r="JZ10" s="25"/>
+      <c r="KA10" s="25"/>
+      <c r="KB10" s="25"/>
+      <c r="KC10" s="25"/>
+      <c r="KD10" s="25"/>
+      <c r="KE10" s="25"/>
+      <c r="KF10" s="25"/>
+      <c r="KG10" s="25"/>
+      <c r="KH10" s="25"/>
+      <c r="KI10" s="25"/>
+      <c r="KJ10" s="25"/>
+      <c r="KK10" s="25"/>
+      <c r="KL10" s="25"/>
+      <c r="KM10" s="25"/>
+      <c r="KN10" s="25"/>
+      <c r="KO10" s="25"/>
+      <c r="KP10" s="25"/>
+      <c r="KQ10" s="25"/>
+      <c r="KR10" s="25"/>
+      <c r="KS10" s="25"/>
+      <c r="KT10" s="25"/>
+      <c r="KU10" s="25"/>
+      <c r="KV10" s="25"/>
+      <c r="KW10" s="25"/>
+      <c r="KX10" s="25"/>
+      <c r="KY10" s="25"/>
+      <c r="KZ10" s="25"/>
+      <c r="LA10" s="25"/>
+      <c r="LB10" s="25"/>
+      <c r="LC10" s="25"/>
+      <c r="LD10" s="25"/>
+      <c r="LE10" s="25"/>
+      <c r="LF10" s="25"/>
+      <c r="LG10" s="25"/>
+      <c r="LH10" s="25"/>
+      <c r="LI10" s="25"/>
+      <c r="LJ10" s="25"/>
+      <c r="LK10" s="25"/>
+      <c r="LL10" s="25"/>
+      <c r="LM10" s="25"/>
+      <c r="LN10" s="25"/>
+      <c r="LO10" s="25"/>
+      <c r="LP10" s="25"/>
+      <c r="LQ10" s="25"/>
+      <c r="LR10" s="25"/>
+      <c r="LS10" s="25"/>
+      <c r="LT10" s="25"/>
+      <c r="LU10" s="25"/>
+      <c r="LV10" s="25"/>
+      <c r="LW10" s="25"/>
+      <c r="LX10" s="25"/>
+      <c r="LY10" s="25"/>
+      <c r="LZ10" s="25"/>
+      <c r="MA10" s="25"/>
+      <c r="MB10" s="25"/>
+      <c r="MC10" s="25"/>
+      <c r="MD10" s="25"/>
+      <c r="ME10" s="25"/>
+      <c r="MF10" s="25"/>
+      <c r="MG10" s="25"/>
+      <c r="MH10" s="25"/>
+      <c r="MI10" s="25"/>
+      <c r="MJ10" s="25"/>
+      <c r="MK10" s="25"/>
+      <c r="ML10" s="25"/>
+      <c r="MM10" s="25"/>
+      <c r="MN10" s="25"/>
+      <c r="MO10" s="25"/>
+      <c r="MP10" s="25"/>
+      <c r="MQ10" s="25"/>
+      <c r="MR10" s="25"/>
+      <c r="MS10" s="25"/>
+      <c r="MT10" s="25"/>
+      <c r="MU10" s="25"/>
+      <c r="MV10" s="25"/>
+      <c r="MW10" s="25"/>
+      <c r="MX10" s="25"/>
+      <c r="MY10" s="25"/>
+      <c r="MZ10" s="25"/>
+      <c r="NA10" s="25"/>
+      <c r="NB10" s="25"/>
+      <c r="NC10" s="25"/>
+      <c r="ND10" s="25"/>
+      <c r="NE10" s="25"/>
+      <c r="NF10" s="25"/>
+      <c r="NG10" s="25"/>
+      <c r="NH10" s="25"/>
+      <c r="NI10" s="25"/>
+      <c r="NJ10" s="25"/>
+      <c r="NK10" s="25"/>
+      <c r="NL10" s="25"/>
+      <c r="NM10" s="25"/>
+      <c r="NN10" s="25"/>
+      <c r="NO10" s="25"/>
+      <c r="NP10" s="25"/>
+      <c r="NQ10" s="25"/>
+      <c r="NR10" s="25"/>
+      <c r="NS10" s="25"/>
+      <c r="NT10" s="25"/>
+      <c r="NU10" s="25"/>
+      <c r="NV10" s="25"/>
+      <c r="NW10" s="25"/>
+      <c r="NX10" s="25"/>
+      <c r="NY10" s="25"/>
+      <c r="NZ10" s="25"/>
+      <c r="OA10" s="25"/>
+      <c r="OB10" s="25"/>
+      <c r="OC10" s="25"/>
+      <c r="OD10" s="25"/>
+      <c r="OE10" s="25"/>
+      <c r="OF10" s="25"/>
+      <c r="OG10" s="25"/>
+      <c r="OH10" s="25"/>
+      <c r="OI10" s="25"/>
+      <c r="OJ10" s="25"/>
+      <c r="OK10" s="25"/>
+      <c r="OL10" s="25"/>
+      <c r="OM10" s="25"/>
+      <c r="ON10" s="25"/>
+      <c r="OO10" s="25"/>
+      <c r="OP10" s="25"/>
+      <c r="OQ10" s="25"/>
+      <c r="OR10" s="25"/>
+      <c r="OS10" s="25"/>
+      <c r="OT10" s="25"/>
+      <c r="OU10" s="25"/>
+      <c r="OV10" s="25"/>
+      <c r="OW10" s="25"/>
+      <c r="OX10" s="25"/>
+      <c r="OY10" s="25"/>
+      <c r="OZ10" s="25"/>
+      <c r="PA10" s="25"/>
+      <c r="PB10" s="25"/>
+      <c r="PC10" s="25"/>
+      <c r="PD10" s="25"/>
+      <c r="PE10" s="25"/>
+      <c r="PF10" s="25"/>
+      <c r="PG10" s="25"/>
+      <c r="PH10" s="25"/>
+      <c r="PI10" s="25"/>
+      <c r="PJ10" s="25"/>
+      <c r="PK10" s="25"/>
+      <c r="PL10" s="25"/>
+      <c r="PM10" s="25"/>
+      <c r="PN10" s="25"/>
+      <c r="PO10" s="25"/>
+      <c r="PP10" s="25"/>
+      <c r="PQ10" s="25"/>
+      <c r="PR10" s="25"/>
+      <c r="PS10" s="25"/>
+      <c r="PT10" s="25"/>
+      <c r="PU10" s="25"/>
+      <c r="PV10" s="25"/>
+      <c r="PW10" s="25"/>
+      <c r="PX10" s="25"/>
+      <c r="PY10" s="25"/>
+      <c r="PZ10" s="25"/>
+      <c r="QA10" s="25"/>
+      <c r="QB10" s="25"/>
+      <c r="QC10" s="25"/>
+      <c r="QD10" s="25"/>
+      <c r="QE10" s="25"/>
+      <c r="QF10" s="25"/>
+      <c r="QG10" s="25"/>
+      <c r="QH10" s="25"/>
+      <c r="QI10" s="25"/>
+      <c r="QJ10" s="25"/>
+      <c r="QK10" s="25"/>
+      <c r="QL10" s="25"/>
+      <c r="QM10" s="25"/>
+      <c r="QN10" s="25"/>
+      <c r="QO10" s="25"/>
+      <c r="QP10" s="25"/>
+      <c r="QQ10" s="25"/>
+      <c r="QR10" s="25"/>
+      <c r="QS10" s="25"/>
+      <c r="QT10" s="25"/>
+      <c r="QU10" s="25"/>
+      <c r="QV10" s="25"/>
+      <c r="QW10" s="25"/>
+      <c r="QX10" s="25"/>
+      <c r="QY10" s="25"/>
+      <c r="QZ10" s="25"/>
+      <c r="RA10" s="25"/>
+      <c r="RB10" s="25"/>
+      <c r="RC10" s="25"/>
+      <c r="RD10" s="25"/>
+      <c r="RE10" s="25"/>
+      <c r="RF10" s="25"/>
+      <c r="RG10" s="25"/>
+      <c r="RH10" s="25"/>
+      <c r="RI10" s="25"/>
+      <c r="RJ10" s="25"/>
+      <c r="RK10" s="25"/>
+      <c r="RL10" s="25"/>
+      <c r="RM10" s="25"/>
+      <c r="RN10" s="25"/>
+      <c r="RO10" s="25"/>
+      <c r="RP10" s="25"/>
+      <c r="RQ10" s="25"/>
+      <c r="RR10" s="25"/>
+      <c r="RS10" s="25"/>
+      <c r="RT10" s="25"/>
+      <c r="RU10" s="25"/>
+      <c r="RV10" s="25"/>
+      <c r="RW10" s="25"/>
+      <c r="RX10" s="25"/>
+      <c r="RY10" s="25"/>
+      <c r="RZ10" s="25"/>
+      <c r="SA10" s="25"/>
+      <c r="SB10" s="25"/>
+      <c r="SC10" s="25"/>
+      <c r="SD10" s="25"/>
+      <c r="SE10" s="25"/>
+      <c r="SF10" s="25"/>
+      <c r="SG10" s="25"/>
+      <c r="SH10" s="25"/>
+      <c r="SI10" s="25"/>
+      <c r="SJ10" s="25"/>
+      <c r="SK10" s="25"/>
+      <c r="SL10" s="25"/>
+      <c r="SM10" s="25"/>
+      <c r="SN10" s="25"/>
+      <c r="SO10" s="25"/>
+      <c r="SP10" s="25"/>
+      <c r="SQ10" s="25"/>
+      <c r="SR10" s="25"/>
+      <c r="SS10" s="25"/>
+      <c r="ST10" s="25"/>
+      <c r="SU10" s="25"/>
+      <c r="SV10" s="25"/>
+      <c r="SW10" s="25"/>
+      <c r="SX10" s="25"/>
+      <c r="SY10" s="25"/>
+      <c r="SZ10" s="25"/>
+      <c r="TA10" s="25"/>
+      <c r="TB10" s="25"/>
+      <c r="TC10" s="25"/>
+      <c r="TD10" s="25"/>
+      <c r="TE10" s="25"/>
+      <c r="TF10" s="25"/>
+      <c r="TG10" s="25"/>
+      <c r="TH10" s="25"/>
+      <c r="TI10" s="25"/>
+      <c r="TJ10" s="25"/>
+      <c r="TK10" s="25"/>
+      <c r="TL10" s="25"/>
+      <c r="TM10" s="25"/>
+      <c r="TN10" s="25"/>
+      <c r="TO10" s="25"/>
+      <c r="TP10" s="25"/>
+      <c r="TQ10" s="25"/>
+      <c r="TR10" s="25"/>
+      <c r="TS10" s="25"/>
+      <c r="TT10" s="25"/>
+      <c r="TU10" s="25"/>
+      <c r="TV10" s="25"/>
+      <c r="TW10" s="25"/>
+      <c r="TX10" s="25"/>
+      <c r="TY10" s="25"/>
+      <c r="TZ10" s="25"/>
+      <c r="UA10" s="25"/>
+      <c r="UB10" s="25"/>
+      <c r="UC10" s="25"/>
+      <c r="UD10" s="25"/>
+      <c r="UE10" s="25"/>
+      <c r="UF10" s="25"/>
+      <c r="UG10" s="25"/>
+      <c r="UH10" s="25"/>
+      <c r="UI10" s="25"/>
+      <c r="UJ10" s="25"/>
+      <c r="UK10" s="25"/>
+      <c r="UL10" s="25"/>
+      <c r="UM10" s="25"/>
+      <c r="UN10" s="25"/>
+      <c r="UO10" s="25"/>
+      <c r="UP10" s="25"/>
+      <c r="UQ10" s="25"/>
+      <c r="UR10" s="25"/>
+      <c r="US10" s="25"/>
+      <c r="UT10" s="25"/>
+      <c r="UU10" s="25"/>
+      <c r="UV10" s="25"/>
+      <c r="UW10" s="25"/>
+      <c r="UX10" s="25"/>
+      <c r="UY10" s="25"/>
+      <c r="UZ10" s="25"/>
+      <c r="VA10" s="25"/>
+      <c r="VB10" s="25"/>
+      <c r="VC10" s="25"/>
+      <c r="VD10" s="25"/>
+      <c r="VE10" s="25"/>
+      <c r="VF10" s="25"/>
+      <c r="VG10" s="25"/>
+      <c r="VH10" s="25"/>
+      <c r="VI10" s="25"/>
+      <c r="VJ10" s="25"/>
+      <c r="VK10" s="25"/>
+      <c r="VL10" s="25"/>
+      <c r="VM10" s="25"/>
+      <c r="VN10" s="25"/>
+      <c r="VO10" s="25"/>
+      <c r="VP10" s="25"/>
+      <c r="VQ10" s="25"/>
+      <c r="VR10" s="25"/>
+      <c r="VS10" s="25"/>
+      <c r="VT10" s="25"/>
+      <c r="VU10" s="25"/>
+      <c r="VV10" s="25"/>
+      <c r="VW10" s="25"/>
+      <c r="VX10" s="25"/>
+      <c r="VY10" s="25"/>
+      <c r="VZ10" s="25"/>
+      <c r="WA10" s="25"/>
+      <c r="WB10" s="25"/>
+      <c r="WC10" s="25"/>
+      <c r="WD10" s="25"/>
+      <c r="WE10" s="25"/>
+      <c r="WF10" s="25"/>
+      <c r="WG10" s="25"/>
+      <c r="WH10" s="25"/>
+      <c r="WI10" s="25"/>
+      <c r="WJ10" s="25"/>
+      <c r="WK10" s="25"/>
+      <c r="WL10" s="25"/>
+      <c r="WM10" s="25"/>
+      <c r="WN10" s="25"/>
+      <c r="WO10" s="25"/>
+      <c r="WP10" s="25"/>
+      <c r="WQ10" s="25"/>
+      <c r="WR10" s="25"/>
+      <c r="WS10" s="25"/>
+      <c r="WT10" s="25"/>
+      <c r="WU10" s="25"/>
+      <c r="WV10" s="25"/>
+      <c r="WW10" s="25"/>
+      <c r="WX10" s="25"/>
+      <c r="WY10" s="25"/>
+      <c r="WZ10" s="25"/>
+      <c r="XA10" s="25"/>
+      <c r="XB10" s="25"/>
+      <c r="XC10" s="25"/>
+      <c r="XD10" s="25"/>
+      <c r="XE10" s="25"/>
+      <c r="XF10" s="25"/>
+      <c r="XG10" s="25"/>
+      <c r="XH10" s="25"/>
+      <c r="XI10" s="25"/>
+      <c r="XJ10" s="25"/>
+      <c r="XK10" s="25"/>
+      <c r="XL10" s="25"/>
+      <c r="XM10" s="25"/>
+      <c r="XN10" s="25"/>
+      <c r="XO10" s="25"/>
+      <c r="XP10" s="25"/>
+      <c r="XQ10" s="25"/>
+      <c r="XR10" s="25"/>
+      <c r="XS10" s="25"/>
+      <c r="XT10" s="25"/>
+      <c r="XU10" s="25"/>
+      <c r="XV10" s="25"/>
+      <c r="XW10" s="25"/>
+      <c r="XX10" s="25"/>
+      <c r="XY10" s="25"/>
+      <c r="XZ10" s="25"/>
+      <c r="YA10" s="25"/>
+      <c r="YB10" s="25"/>
+      <c r="YC10" s="25"/>
+      <c r="YD10" s="25"/>
+      <c r="YE10" s="25"/>
+      <c r="YF10" s="25"/>
+      <c r="YG10" s="25"/>
+      <c r="YH10" s="25"/>
+      <c r="YI10" s="25"/>
+      <c r="YJ10" s="25"/>
+      <c r="YK10" s="25"/>
+      <c r="YL10" s="25"/>
+      <c r="YM10" s="25"/>
+      <c r="YN10" s="25"/>
+      <c r="YO10" s="25"/>
+      <c r="YP10" s="25"/>
+      <c r="YQ10" s="25"/>
+      <c r="YR10" s="25"/>
+      <c r="YS10" s="25"/>
+      <c r="YT10" s="25"/>
+      <c r="YU10" s="25"/>
+      <c r="YV10" s="25"/>
+      <c r="YW10" s="25"/>
+      <c r="YX10" s="25"/>
+      <c r="YY10" s="25"/>
+      <c r="YZ10" s="25"/>
+      <c r="ZA10" s="25"/>
+      <c r="ZB10" s="25"/>
+      <c r="ZC10" s="25"/>
+      <c r="ZD10" s="25"/>
+      <c r="ZE10" s="25"/>
+      <c r="ZF10" s="25"/>
+      <c r="ZG10" s="25"/>
+      <c r="ZH10" s="25"/>
+      <c r="ZI10" s="25"/>
+      <c r="ZJ10" s="25"/>
+      <c r="ZK10" s="25"/>
+      <c r="ZL10" s="25"/>
+      <c r="ZM10" s="25"/>
+      <c r="ZN10" s="25"/>
+      <c r="ZO10" s="25"/>
+      <c r="ZP10" s="25"/>
+      <c r="ZQ10" s="25"/>
+      <c r="ZR10" s="25"/>
+      <c r="ZS10" s="25"/>
+      <c r="ZT10" s="25"/>
+      <c r="ZU10" s="25"/>
+      <c r="ZV10" s="25"/>
+      <c r="ZW10" s="25"/>
+      <c r="ZX10" s="25"/>
+      <c r="ZY10" s="25"/>
+      <c r="ZZ10" s="25"/>
+      <c r="AAA10" s="25"/>
+      <c r="AAB10" s="25"/>
+      <c r="AAC10" s="25"/>
+      <c r="AAD10" s="25"/>
+      <c r="AAE10" s="25"/>
+      <c r="AAF10" s="25"/>
+      <c r="AAG10" s="25"/>
+      <c r="AAH10" s="25"/>
+      <c r="AAI10" s="25"/>
+      <c r="AAJ10" s="25"/>
+      <c r="AAK10" s="25"/>
+      <c r="AAL10" s="25"/>
+      <c r="AAM10" s="25"/>
+      <c r="AAN10" s="25"/>
+      <c r="AAO10" s="25"/>
+      <c r="AAP10" s="25"/>
+      <c r="AAQ10" s="25"/>
+      <c r="AAR10" s="25"/>
+      <c r="AAS10" s="25"/>
+      <c r="AAT10" s="25"/>
+      <c r="AAU10" s="25"/>
+      <c r="AAV10" s="25"/>
+      <c r="AAW10" s="25"/>
+      <c r="AAX10" s="25"/>
+      <c r="AAY10" s="25"/>
+      <c r="AAZ10" s="25"/>
+      <c r="ABA10" s="25"/>
+      <c r="ABB10" s="25"/>
+      <c r="ABC10" s="25"/>
+      <c r="ABD10" s="25"/>
+      <c r="ABE10" s="25"/>
+      <c r="ABF10" s="25"/>
+      <c r="ABG10" s="25"/>
+      <c r="ABH10" s="25"/>
+      <c r="ABI10" s="25"/>
+      <c r="ABJ10" s="25"/>
+      <c r="ABK10" s="25"/>
+      <c r="ABL10" s="25"/>
+      <c r="ABM10" s="25"/>
+      <c r="ABN10" s="25"/>
+      <c r="ABO10" s="25"/>
+      <c r="ABP10" s="25"/>
+      <c r="ABQ10" s="25"/>
+      <c r="ABR10" s="25"/>
+      <c r="ABS10" s="25"/>
+      <c r="ABT10" s="25"/>
+      <c r="ABU10" s="25"/>
+      <c r="ABV10" s="25"/>
+      <c r="ABW10" s="25"/>
+      <c r="ABX10" s="25"/>
+      <c r="ABY10" s="25"/>
+      <c r="ABZ10" s="25"/>
+      <c r="ACA10" s="25"/>
+      <c r="ACB10" s="25"/>
+      <c r="ACC10" s="25"/>
+      <c r="ACD10" s="25"/>
+      <c r="ACE10" s="25"/>
+      <c r="ACF10" s="25"/>
+      <c r="ACG10" s="25"/>
+      <c r="ACH10" s="25"/>
+      <c r="ACI10" s="25"/>
+      <c r="ACJ10" s="25"/>
+      <c r="ACK10" s="25"/>
+      <c r="ACL10" s="25"/>
+      <c r="ACM10" s="25"/>
+      <c r="ACN10" s="25"/>
+      <c r="ACO10" s="25"/>
+      <c r="ACP10" s="25"/>
+      <c r="ACQ10" s="25"/>
+      <c r="ACR10" s="25"/>
+      <c r="ACS10" s="25"/>
+      <c r="ACT10" s="25"/>
+      <c r="ACU10" s="25"/>
+      <c r="ACV10" s="25"/>
+      <c r="ACW10" s="25"/>
+      <c r="ACX10" s="25"/>
+      <c r="ACY10" s="25"/>
+      <c r="ACZ10" s="25"/>
+      <c r="ADA10" s="25"/>
+      <c r="ADB10" s="25"/>
+      <c r="ADC10" s="25"/>
+      <c r="ADD10" s="25"/>
+      <c r="ADE10" s="25"/>
+      <c r="ADF10" s="25"/>
+      <c r="ADG10" s="25"/>
+      <c r="ADH10" s="25"/>
+      <c r="ADI10" s="25"/>
+      <c r="ADJ10" s="25"/>
+      <c r="ADK10" s="25"/>
+      <c r="ADL10" s="25"/>
+      <c r="ADM10" s="25"/>
+      <c r="ADN10" s="25"/>
+      <c r="ADO10" s="25"/>
+      <c r="ADP10" s="25"/>
+      <c r="ADQ10" s="25"/>
+      <c r="ADR10" s="25"/>
+      <c r="ADS10" s="25"/>
+      <c r="ADT10" s="25"/>
+      <c r="ADU10" s="25"/>
+      <c r="ADV10" s="25"/>
+      <c r="ADW10" s="25"/>
+      <c r="ADX10" s="25"/>
+      <c r="ADY10" s="25"/>
+      <c r="ADZ10" s="25"/>
+      <c r="AEA10" s="25"/>
+      <c r="AEB10" s="25"/>
+      <c r="AEC10" s="25"/>
+      <c r="AED10" s="25"/>
+      <c r="AEE10" s="25"/>
+      <c r="AEF10" s="25"/>
+      <c r="AEG10" s="25"/>
+      <c r="AEH10" s="25"/>
+      <c r="AEI10" s="25"/>
+      <c r="AEJ10" s="25"/>
+      <c r="AEK10" s="25"/>
+      <c r="AEL10" s="25"/>
+      <c r="AEM10" s="25"/>
+      <c r="AEN10" s="25"/>
+      <c r="AEO10" s="25"/>
+      <c r="AEP10" s="25"/>
+      <c r="AEQ10" s="25"/>
+      <c r="AER10" s="25"/>
+      <c r="AES10" s="25"/>
+      <c r="AET10" s="25"/>
+      <c r="AEU10" s="25"/>
+      <c r="AEV10" s="25"/>
+      <c r="AEW10" s="25"/>
+      <c r="AEX10" s="25"/>
+      <c r="AEY10" s="25"/>
+      <c r="AEZ10" s="25"/>
+      <c r="AFA10" s="25"/>
+      <c r="AFB10" s="25"/>
+      <c r="AFC10" s="25"/>
+      <c r="AFD10" s="25"/>
+      <c r="AFE10" s="25"/>
+      <c r="AFF10" s="25"/>
+      <c r="AFG10" s="25"/>
+      <c r="AFH10" s="25"/>
+      <c r="AFI10" s="25"/>
+      <c r="AFJ10" s="25"/>
+      <c r="AFK10" s="25"/>
+      <c r="AFL10" s="25"/>
+      <c r="AFM10" s="25"/>
+      <c r="AFN10" s="25"/>
+      <c r="AFO10" s="25"/>
+      <c r="AFP10" s="25"/>
+      <c r="AFQ10" s="25"/>
+      <c r="AFR10" s="25"/>
+      <c r="AFS10" s="25"/>
+      <c r="AFT10" s="25"/>
+      <c r="AFU10" s="25"/>
+      <c r="AFV10" s="25"/>
+      <c r="AFW10" s="25"/>
+      <c r="AFX10" s="25"/>
+      <c r="AFY10" s="25"/>
+      <c r="AFZ10" s="25"/>
+      <c r="AGA10" s="25"/>
+      <c r="AGB10" s="25"/>
+      <c r="AGC10" s="25"/>
+      <c r="AGD10" s="25"/>
+      <c r="AGE10" s="25"/>
+      <c r="AGF10" s="25"/>
+      <c r="AGG10" s="25"/>
+      <c r="AGH10" s="25"/>
+      <c r="AGI10" s="25"/>
+      <c r="AGJ10" s="25"/>
+      <c r="AGK10" s="25"/>
+      <c r="AGL10" s="25"/>
+      <c r="AGM10" s="25"/>
+      <c r="AGN10" s="25"/>
+      <c r="AGO10" s="25"/>
+      <c r="AGP10" s="25"/>
+      <c r="AGQ10" s="25"/>
+      <c r="AGR10" s="25"/>
+      <c r="AGS10" s="25"/>
+      <c r="AGT10" s="25"/>
+      <c r="AGU10" s="25"/>
+      <c r="AGV10" s="25"/>
+      <c r="AGW10" s="25"/>
+      <c r="AGX10" s="25"/>
+      <c r="AGY10" s="25"/>
+      <c r="AGZ10" s="25"/>
+      <c r="AHA10" s="25"/>
+      <c r="AHB10" s="25"/>
+      <c r="AHC10" s="25"/>
+      <c r="AHD10" s="25"/>
+      <c r="AHE10" s="25"/>
+      <c r="AHF10" s="25"/>
+      <c r="AHG10" s="25"/>
+      <c r="AHH10" s="25"/>
+      <c r="AHI10" s="25"/>
+      <c r="AHJ10" s="25"/>
+      <c r="AHK10" s="25"/>
+      <c r="AHL10" s="25"/>
+      <c r="AHM10" s="25"/>
+      <c r="AHN10" s="25"/>
+      <c r="AHO10" s="25"/>
+      <c r="AHP10" s="25"/>
+      <c r="AHQ10" s="25"/>
+      <c r="AHR10" s="25"/>
+      <c r="AHS10" s="25"/>
+      <c r="AHT10" s="25"/>
+      <c r="AHU10" s="25"/>
+      <c r="AHV10" s="25"/>
+      <c r="AHW10" s="25"/>
+      <c r="AHX10" s="25"/>
+      <c r="AHY10" s="25"/>
+      <c r="AHZ10" s="25"/>
+      <c r="AIA10" s="25"/>
+      <c r="AIB10" s="25"/>
+      <c r="AIC10" s="25"/>
+      <c r="AID10" s="25"/>
+      <c r="AIE10" s="25"/>
+      <c r="AIF10" s="25"/>
+      <c r="AIG10" s="25"/>
+      <c r="AIH10" s="25"/>
+      <c r="AII10" s="25"/>
+      <c r="AIJ10" s="25"/>
+      <c r="AIK10" s="25"/>
+      <c r="AIL10" s="25"/>
+      <c r="AIM10" s="25"/>
+      <c r="AIN10" s="25"/>
+      <c r="AIO10" s="25"/>
+      <c r="AIP10" s="25"/>
+      <c r="AIQ10" s="25"/>
+      <c r="AIR10" s="25"/>
+      <c r="AIS10" s="25"/>
+      <c r="AIT10" s="25"/>
+      <c r="AIU10" s="25"/>
+      <c r="AIV10" s="25"/>
+      <c r="AIW10" s="25"/>
+      <c r="AIX10" s="25"/>
+      <c r="AIY10" s="25"/>
+      <c r="AIZ10" s="25"/>
+      <c r="AJA10" s="25"/>
+      <c r="AJB10" s="25"/>
+      <c r="AJC10" s="25"/>
+      <c r="AJD10" s="25"/>
+      <c r="AJE10" s="25"/>
+      <c r="AJF10" s="25"/>
+      <c r="AJG10" s="25"/>
+      <c r="AJH10" s="25"/>
+      <c r="AJI10" s="25"/>
+      <c r="AJJ10" s="25"/>
+      <c r="AJK10" s="25"/>
+      <c r="AJL10" s="25"/>
+      <c r="AJM10" s="25"/>
+      <c r="AJN10" s="25"/>
+      <c r="AJO10" s="25"/>
+      <c r="AJP10" s="25"/>
+      <c r="AJQ10" s="25"/>
+      <c r="AJR10" s="25"/>
+      <c r="AJS10" s="25"/>
+      <c r="AJT10" s="25"/>
+      <c r="AJU10" s="25"/>
+      <c r="AJV10" s="25"/>
+      <c r="AJW10" s="25"/>
+      <c r="AJX10" s="25"/>
+      <c r="AJY10" s="25"/>
+      <c r="AJZ10" s="25"/>
+      <c r="AKA10" s="25"/>
+      <c r="AKB10" s="25"/>
+      <c r="AKC10" s="25"/>
+      <c r="AKD10" s="25"/>
+      <c r="AKE10" s="25"/>
+      <c r="AKF10" s="25"/>
+      <c r="AKG10" s="25"/>
+      <c r="AKH10" s="25"/>
+      <c r="AKI10" s="25"/>
+      <c r="AKJ10" s="25"/>
+      <c r="AKK10" s="25"/>
+      <c r="AKL10" s="25"/>
+      <c r="AKM10" s="25"/>
+      <c r="AKN10" s="25"/>
+      <c r="AKO10" s="25"/>
+      <c r="AKP10" s="25"/>
+      <c r="AKQ10" s="25"/>
+      <c r="AKR10" s="25"/>
+      <c r="AKS10" s="25"/>
+      <c r="AKT10" s="25"/>
+      <c r="AKU10" s="25"/>
+      <c r="AKV10" s="25"/>
+      <c r="AKW10" s="25"/>
+      <c r="AKX10" s="25"/>
+      <c r="AKY10" s="25"/>
+      <c r="AKZ10" s="25"/>
+      <c r="ALA10" s="25"/>
+      <c r="ALB10" s="25"/>
+      <c r="ALC10" s="25"/>
+      <c r="ALD10" s="25"/>
+      <c r="ALE10" s="25"/>
+      <c r="ALF10" s="25"/>
+      <c r="ALG10" s="25"/>
+      <c r="ALH10" s="25"/>
+      <c r="ALI10" s="25"/>
+      <c r="ALJ10" s="25"/>
+      <c r="ALK10" s="25"/>
+      <c r="ALL10" s="25"/>
+      <c r="ALM10" s="25"/>
+      <c r="ALN10" s="25"/>
+      <c r="ALO10" s="25"/>
+      <c r="ALP10" s="25"/>
+      <c r="ALQ10" s="25"/>
+      <c r="ALR10" s="25"/>
+      <c r="ALS10" s="25"/>
+      <c r="ALT10" s="25"/>
+      <c r="ALU10" s="25"/>
+      <c r="ALV10" s="25"/>
+      <c r="ALW10" s="25"/>
+      <c r="ALX10" s="25"/>
+      <c r="ALY10" s="25"/>
+      <c r="ALZ10" s="25"/>
+      <c r="AMA10" s="25"/>
+      <c r="AMB10" s="25"/>
+      <c r="AMC10" s="25"/>
+      <c r="AMD10" s="25"/>
+      <c r="AME10" s="25"/>
+      <c r="AMF10" s="25"/>
+      <c r="AMG10" s="25"/>
+      <c r="AMH10" s="25"/>
+      <c r="AMI10" s="25"/>
+      <c r="AMJ10" s="25"/>
+    </row>
+    <row r="11" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1332,7 +3408,7 @@
       <c r="E11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <v>42282</v>
       </c>
       <c r="G11" s="5">
@@ -1341,10 +3417,10 @@
       <c r="H11" s="6">
         <v>1</v>
       </c>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1356,7 +3432,7 @@
       <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="19">
         <v>42282</v>
       </c>
       <c r="G12" s="5">
@@ -1365,10 +3441,10 @@
       <c r="H12" s="6">
         <v>1</v>
       </c>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1380,7 +3456,7 @@
       <c r="E13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="19">
         <v>42282</v>
       </c>
       <c r="G13" s="5">
@@ -1389,37 +3465,1053 @@
       <c r="H13" s="6">
         <v>1</v>
       </c>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:1024" s="32" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="5">
+      <c r="F14" s="34"/>
+      <c r="G14" s="29">
         <v>42286</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="30">
         <v>0</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="35" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="25"/>
+      <c r="AD14" s="25"/>
+      <c r="AE14" s="25"/>
+      <c r="AF14" s="25"/>
+      <c r="AG14" s="25"/>
+      <c r="AH14" s="25"/>
+      <c r="AI14" s="25"/>
+      <c r="AJ14" s="25"/>
+      <c r="AK14" s="25"/>
+      <c r="AL14" s="25"/>
+      <c r="AM14" s="25"/>
+      <c r="AN14" s="25"/>
+      <c r="AO14" s="25"/>
+      <c r="AP14" s="25"/>
+      <c r="AQ14" s="25"/>
+      <c r="AR14" s="25"/>
+      <c r="AS14" s="25"/>
+      <c r="AT14" s="25"/>
+      <c r="AU14" s="25"/>
+      <c r="AV14" s="25"/>
+      <c r="AW14" s="25"/>
+      <c r="AX14" s="25"/>
+      <c r="AY14" s="25"/>
+      <c r="AZ14" s="25"/>
+      <c r="BA14" s="25"/>
+      <c r="BB14" s="25"/>
+      <c r="BC14" s="25"/>
+      <c r="BD14" s="25"/>
+      <c r="BE14" s="25"/>
+      <c r="BF14" s="25"/>
+      <c r="BG14" s="25"/>
+      <c r="BH14" s="25"/>
+      <c r="BI14" s="25"/>
+      <c r="BJ14" s="25"/>
+      <c r="BK14" s="25"/>
+      <c r="BL14" s="25"/>
+      <c r="BM14" s="25"/>
+      <c r="BN14" s="25"/>
+      <c r="BO14" s="25"/>
+      <c r="BP14" s="25"/>
+      <c r="BQ14" s="25"/>
+      <c r="BR14" s="25"/>
+      <c r="BS14" s="25"/>
+      <c r="BT14" s="25"/>
+      <c r="BU14" s="25"/>
+      <c r="BV14" s="25"/>
+      <c r="BW14" s="25"/>
+      <c r="BX14" s="25"/>
+      <c r="BY14" s="25"/>
+      <c r="BZ14" s="25"/>
+      <c r="CA14" s="25"/>
+      <c r="CB14" s="25"/>
+      <c r="CC14" s="25"/>
+      <c r="CD14" s="25"/>
+      <c r="CE14" s="25"/>
+      <c r="CF14" s="25"/>
+      <c r="CG14" s="25"/>
+      <c r="CH14" s="25"/>
+      <c r="CI14" s="25"/>
+      <c r="CJ14" s="25"/>
+      <c r="CK14" s="25"/>
+      <c r="CL14" s="25"/>
+      <c r="CM14" s="25"/>
+      <c r="CN14" s="25"/>
+      <c r="CO14" s="25"/>
+      <c r="CP14" s="25"/>
+      <c r="CQ14" s="25"/>
+      <c r="CR14" s="25"/>
+      <c r="CS14" s="25"/>
+      <c r="CT14" s="25"/>
+      <c r="CU14" s="25"/>
+      <c r="CV14" s="25"/>
+      <c r="CW14" s="25"/>
+      <c r="CX14" s="25"/>
+      <c r="CY14" s="25"/>
+      <c r="CZ14" s="25"/>
+      <c r="DA14" s="25"/>
+      <c r="DB14" s="25"/>
+      <c r="DC14" s="25"/>
+      <c r="DD14" s="25"/>
+      <c r="DE14" s="25"/>
+      <c r="DF14" s="25"/>
+      <c r="DG14" s="25"/>
+      <c r="DH14" s="25"/>
+      <c r="DI14" s="25"/>
+      <c r="DJ14" s="25"/>
+      <c r="DK14" s="25"/>
+      <c r="DL14" s="25"/>
+      <c r="DM14" s="25"/>
+      <c r="DN14" s="25"/>
+      <c r="DO14" s="25"/>
+      <c r="DP14" s="25"/>
+      <c r="DQ14" s="25"/>
+      <c r="DR14" s="25"/>
+      <c r="DS14" s="25"/>
+      <c r="DT14" s="25"/>
+      <c r="DU14" s="25"/>
+      <c r="DV14" s="25"/>
+      <c r="DW14" s="25"/>
+      <c r="DX14" s="25"/>
+      <c r="DY14" s="25"/>
+      <c r="DZ14" s="25"/>
+      <c r="EA14" s="25"/>
+      <c r="EB14" s="25"/>
+      <c r="EC14" s="25"/>
+      <c r="ED14" s="25"/>
+      <c r="EE14" s="25"/>
+      <c r="EF14" s="25"/>
+      <c r="EG14" s="25"/>
+      <c r="EH14" s="25"/>
+      <c r="EI14" s="25"/>
+      <c r="EJ14" s="25"/>
+      <c r="EK14" s="25"/>
+      <c r="EL14" s="25"/>
+      <c r="EM14" s="25"/>
+      <c r="EN14" s="25"/>
+      <c r="EO14" s="25"/>
+      <c r="EP14" s="25"/>
+      <c r="EQ14" s="25"/>
+      <c r="ER14" s="25"/>
+      <c r="ES14" s="25"/>
+      <c r="ET14" s="25"/>
+      <c r="EU14" s="25"/>
+      <c r="EV14" s="25"/>
+      <c r="EW14" s="25"/>
+      <c r="EX14" s="25"/>
+      <c r="EY14" s="25"/>
+      <c r="EZ14" s="25"/>
+      <c r="FA14" s="25"/>
+      <c r="FB14" s="25"/>
+      <c r="FC14" s="25"/>
+      <c r="FD14" s="25"/>
+      <c r="FE14" s="25"/>
+      <c r="FF14" s="25"/>
+      <c r="FG14" s="25"/>
+      <c r="FH14" s="25"/>
+      <c r="FI14" s="25"/>
+      <c r="FJ14" s="25"/>
+      <c r="FK14" s="25"/>
+      <c r="FL14" s="25"/>
+      <c r="FM14" s="25"/>
+      <c r="FN14" s="25"/>
+      <c r="FO14" s="25"/>
+      <c r="FP14" s="25"/>
+      <c r="FQ14" s="25"/>
+      <c r="FR14" s="25"/>
+      <c r="FS14" s="25"/>
+      <c r="FT14" s="25"/>
+      <c r="FU14" s="25"/>
+      <c r="FV14" s="25"/>
+      <c r="FW14" s="25"/>
+      <c r="FX14" s="25"/>
+      <c r="FY14" s="25"/>
+      <c r="FZ14" s="25"/>
+      <c r="GA14" s="25"/>
+      <c r="GB14" s="25"/>
+      <c r="GC14" s="25"/>
+      <c r="GD14" s="25"/>
+      <c r="GE14" s="25"/>
+      <c r="GF14" s="25"/>
+      <c r="GG14" s="25"/>
+      <c r="GH14" s="25"/>
+      <c r="GI14" s="25"/>
+      <c r="GJ14" s="25"/>
+      <c r="GK14" s="25"/>
+      <c r="GL14" s="25"/>
+      <c r="GM14" s="25"/>
+      <c r="GN14" s="25"/>
+      <c r="GO14" s="25"/>
+      <c r="GP14" s="25"/>
+      <c r="GQ14" s="25"/>
+      <c r="GR14" s="25"/>
+      <c r="GS14" s="25"/>
+      <c r="GT14" s="25"/>
+      <c r="GU14" s="25"/>
+      <c r="GV14" s="25"/>
+      <c r="GW14" s="25"/>
+      <c r="GX14" s="25"/>
+      <c r="GY14" s="25"/>
+      <c r="GZ14" s="25"/>
+      <c r="HA14" s="25"/>
+      <c r="HB14" s="25"/>
+      <c r="HC14" s="25"/>
+      <c r="HD14" s="25"/>
+      <c r="HE14" s="25"/>
+      <c r="HF14" s="25"/>
+      <c r="HG14" s="25"/>
+      <c r="HH14" s="25"/>
+      <c r="HI14" s="25"/>
+      <c r="HJ14" s="25"/>
+      <c r="HK14" s="25"/>
+      <c r="HL14" s="25"/>
+      <c r="HM14" s="25"/>
+      <c r="HN14" s="25"/>
+      <c r="HO14" s="25"/>
+      <c r="HP14" s="25"/>
+      <c r="HQ14" s="25"/>
+      <c r="HR14" s="25"/>
+      <c r="HS14" s="25"/>
+      <c r="HT14" s="25"/>
+      <c r="HU14" s="25"/>
+      <c r="HV14" s="25"/>
+      <c r="HW14" s="25"/>
+      <c r="HX14" s="25"/>
+      <c r="HY14" s="25"/>
+      <c r="HZ14" s="25"/>
+      <c r="IA14" s="25"/>
+      <c r="IB14" s="25"/>
+      <c r="IC14" s="25"/>
+      <c r="ID14" s="25"/>
+      <c r="IE14" s="25"/>
+      <c r="IF14" s="25"/>
+      <c r="IG14" s="25"/>
+      <c r="IH14" s="25"/>
+      <c r="II14" s="25"/>
+      <c r="IJ14" s="25"/>
+      <c r="IK14" s="25"/>
+      <c r="IL14" s="25"/>
+      <c r="IM14" s="25"/>
+      <c r="IN14" s="25"/>
+      <c r="IO14" s="25"/>
+      <c r="IP14" s="25"/>
+      <c r="IQ14" s="25"/>
+      <c r="IR14" s="25"/>
+      <c r="IS14" s="25"/>
+      <c r="IT14" s="25"/>
+      <c r="IU14" s="25"/>
+      <c r="IV14" s="25"/>
+      <c r="IW14" s="25"/>
+      <c r="IX14" s="25"/>
+      <c r="IY14" s="25"/>
+      <c r="IZ14" s="25"/>
+      <c r="JA14" s="25"/>
+      <c r="JB14" s="25"/>
+      <c r="JC14" s="25"/>
+      <c r="JD14" s="25"/>
+      <c r="JE14" s="25"/>
+      <c r="JF14" s="25"/>
+      <c r="JG14" s="25"/>
+      <c r="JH14" s="25"/>
+      <c r="JI14" s="25"/>
+      <c r="JJ14" s="25"/>
+      <c r="JK14" s="25"/>
+      <c r="JL14" s="25"/>
+      <c r="JM14" s="25"/>
+      <c r="JN14" s="25"/>
+      <c r="JO14" s="25"/>
+      <c r="JP14" s="25"/>
+      <c r="JQ14" s="25"/>
+      <c r="JR14" s="25"/>
+      <c r="JS14" s="25"/>
+      <c r="JT14" s="25"/>
+      <c r="JU14" s="25"/>
+      <c r="JV14" s="25"/>
+      <c r="JW14" s="25"/>
+      <c r="JX14" s="25"/>
+      <c r="JY14" s="25"/>
+      <c r="JZ14" s="25"/>
+      <c r="KA14" s="25"/>
+      <c r="KB14" s="25"/>
+      <c r="KC14" s="25"/>
+      <c r="KD14" s="25"/>
+      <c r="KE14" s="25"/>
+      <c r="KF14" s="25"/>
+      <c r="KG14" s="25"/>
+      <c r="KH14" s="25"/>
+      <c r="KI14" s="25"/>
+      <c r="KJ14" s="25"/>
+      <c r="KK14" s="25"/>
+      <c r="KL14" s="25"/>
+      <c r="KM14" s="25"/>
+      <c r="KN14" s="25"/>
+      <c r="KO14" s="25"/>
+      <c r="KP14" s="25"/>
+      <c r="KQ14" s="25"/>
+      <c r="KR14" s="25"/>
+      <c r="KS14" s="25"/>
+      <c r="KT14" s="25"/>
+      <c r="KU14" s="25"/>
+      <c r="KV14" s="25"/>
+      <c r="KW14" s="25"/>
+      <c r="KX14" s="25"/>
+      <c r="KY14" s="25"/>
+      <c r="KZ14" s="25"/>
+      <c r="LA14" s="25"/>
+      <c r="LB14" s="25"/>
+      <c r="LC14" s="25"/>
+      <c r="LD14" s="25"/>
+      <c r="LE14" s="25"/>
+      <c r="LF14" s="25"/>
+      <c r="LG14" s="25"/>
+      <c r="LH14" s="25"/>
+      <c r="LI14" s="25"/>
+      <c r="LJ14" s="25"/>
+      <c r="LK14" s="25"/>
+      <c r="LL14" s="25"/>
+      <c r="LM14" s="25"/>
+      <c r="LN14" s="25"/>
+      <c r="LO14" s="25"/>
+      <c r="LP14" s="25"/>
+      <c r="LQ14" s="25"/>
+      <c r="LR14" s="25"/>
+      <c r="LS14" s="25"/>
+      <c r="LT14" s="25"/>
+      <c r="LU14" s="25"/>
+      <c r="LV14" s="25"/>
+      <c r="LW14" s="25"/>
+      <c r="LX14" s="25"/>
+      <c r="LY14" s="25"/>
+      <c r="LZ14" s="25"/>
+      <c r="MA14" s="25"/>
+      <c r="MB14" s="25"/>
+      <c r="MC14" s="25"/>
+      <c r="MD14" s="25"/>
+      <c r="ME14" s="25"/>
+      <c r="MF14" s="25"/>
+      <c r="MG14" s="25"/>
+      <c r="MH14" s="25"/>
+      <c r="MI14" s="25"/>
+      <c r="MJ14" s="25"/>
+      <c r="MK14" s="25"/>
+      <c r="ML14" s="25"/>
+      <c r="MM14" s="25"/>
+      <c r="MN14" s="25"/>
+      <c r="MO14" s="25"/>
+      <c r="MP14" s="25"/>
+      <c r="MQ14" s="25"/>
+      <c r="MR14" s="25"/>
+      <c r="MS14" s="25"/>
+      <c r="MT14" s="25"/>
+      <c r="MU14" s="25"/>
+      <c r="MV14" s="25"/>
+      <c r="MW14" s="25"/>
+      <c r="MX14" s="25"/>
+      <c r="MY14" s="25"/>
+      <c r="MZ14" s="25"/>
+      <c r="NA14" s="25"/>
+      <c r="NB14" s="25"/>
+      <c r="NC14" s="25"/>
+      <c r="ND14" s="25"/>
+      <c r="NE14" s="25"/>
+      <c r="NF14" s="25"/>
+      <c r="NG14" s="25"/>
+      <c r="NH14" s="25"/>
+      <c r="NI14" s="25"/>
+      <c r="NJ14" s="25"/>
+      <c r="NK14" s="25"/>
+      <c r="NL14" s="25"/>
+      <c r="NM14" s="25"/>
+      <c r="NN14" s="25"/>
+      <c r="NO14" s="25"/>
+      <c r="NP14" s="25"/>
+      <c r="NQ14" s="25"/>
+      <c r="NR14" s="25"/>
+      <c r="NS14" s="25"/>
+      <c r="NT14" s="25"/>
+      <c r="NU14" s="25"/>
+      <c r="NV14" s="25"/>
+      <c r="NW14" s="25"/>
+      <c r="NX14" s="25"/>
+      <c r="NY14" s="25"/>
+      <c r="NZ14" s="25"/>
+      <c r="OA14" s="25"/>
+      <c r="OB14" s="25"/>
+      <c r="OC14" s="25"/>
+      <c r="OD14" s="25"/>
+      <c r="OE14" s="25"/>
+      <c r="OF14" s="25"/>
+      <c r="OG14" s="25"/>
+      <c r="OH14" s="25"/>
+      <c r="OI14" s="25"/>
+      <c r="OJ14" s="25"/>
+      <c r="OK14" s="25"/>
+      <c r="OL14" s="25"/>
+      <c r="OM14" s="25"/>
+      <c r="ON14" s="25"/>
+      <c r="OO14" s="25"/>
+      <c r="OP14" s="25"/>
+      <c r="OQ14" s="25"/>
+      <c r="OR14" s="25"/>
+      <c r="OS14" s="25"/>
+      <c r="OT14" s="25"/>
+      <c r="OU14" s="25"/>
+      <c r="OV14" s="25"/>
+      <c r="OW14" s="25"/>
+      <c r="OX14" s="25"/>
+      <c r="OY14" s="25"/>
+      <c r="OZ14" s="25"/>
+      <c r="PA14" s="25"/>
+      <c r="PB14" s="25"/>
+      <c r="PC14" s="25"/>
+      <c r="PD14" s="25"/>
+      <c r="PE14" s="25"/>
+      <c r="PF14" s="25"/>
+      <c r="PG14" s="25"/>
+      <c r="PH14" s="25"/>
+      <c r="PI14" s="25"/>
+      <c r="PJ14" s="25"/>
+      <c r="PK14" s="25"/>
+      <c r="PL14" s="25"/>
+      <c r="PM14" s="25"/>
+      <c r="PN14" s="25"/>
+      <c r="PO14" s="25"/>
+      <c r="PP14" s="25"/>
+      <c r="PQ14" s="25"/>
+      <c r="PR14" s="25"/>
+      <c r="PS14" s="25"/>
+      <c r="PT14" s="25"/>
+      <c r="PU14" s="25"/>
+      <c r="PV14" s="25"/>
+      <c r="PW14" s="25"/>
+      <c r="PX14" s="25"/>
+      <c r="PY14" s="25"/>
+      <c r="PZ14" s="25"/>
+      <c r="QA14" s="25"/>
+      <c r="QB14" s="25"/>
+      <c r="QC14" s="25"/>
+      <c r="QD14" s="25"/>
+      <c r="QE14" s="25"/>
+      <c r="QF14" s="25"/>
+      <c r="QG14" s="25"/>
+      <c r="QH14" s="25"/>
+      <c r="QI14" s="25"/>
+      <c r="QJ14" s="25"/>
+      <c r="QK14" s="25"/>
+      <c r="QL14" s="25"/>
+      <c r="QM14" s="25"/>
+      <c r="QN14" s="25"/>
+      <c r="QO14" s="25"/>
+      <c r="QP14" s="25"/>
+      <c r="QQ14" s="25"/>
+      <c r="QR14" s="25"/>
+      <c r="QS14" s="25"/>
+      <c r="QT14" s="25"/>
+      <c r="QU14" s="25"/>
+      <c r="QV14" s="25"/>
+      <c r="QW14" s="25"/>
+      <c r="QX14" s="25"/>
+      <c r="QY14" s="25"/>
+      <c r="QZ14" s="25"/>
+      <c r="RA14" s="25"/>
+      <c r="RB14" s="25"/>
+      <c r="RC14" s="25"/>
+      <c r="RD14" s="25"/>
+      <c r="RE14" s="25"/>
+      <c r="RF14" s="25"/>
+      <c r="RG14" s="25"/>
+      <c r="RH14" s="25"/>
+      <c r="RI14" s="25"/>
+      <c r="RJ14" s="25"/>
+      <c r="RK14" s="25"/>
+      <c r="RL14" s="25"/>
+      <c r="RM14" s="25"/>
+      <c r="RN14" s="25"/>
+      <c r="RO14" s="25"/>
+      <c r="RP14" s="25"/>
+      <c r="RQ14" s="25"/>
+      <c r="RR14" s="25"/>
+      <c r="RS14" s="25"/>
+      <c r="RT14" s="25"/>
+      <c r="RU14" s="25"/>
+      <c r="RV14" s="25"/>
+      <c r="RW14" s="25"/>
+      <c r="RX14" s="25"/>
+      <c r="RY14" s="25"/>
+      <c r="RZ14" s="25"/>
+      <c r="SA14" s="25"/>
+      <c r="SB14" s="25"/>
+      <c r="SC14" s="25"/>
+      <c r="SD14" s="25"/>
+      <c r="SE14" s="25"/>
+      <c r="SF14" s="25"/>
+      <c r="SG14" s="25"/>
+      <c r="SH14" s="25"/>
+      <c r="SI14" s="25"/>
+      <c r="SJ14" s="25"/>
+      <c r="SK14" s="25"/>
+      <c r="SL14" s="25"/>
+      <c r="SM14" s="25"/>
+      <c r="SN14" s="25"/>
+      <c r="SO14" s="25"/>
+      <c r="SP14" s="25"/>
+      <c r="SQ14" s="25"/>
+      <c r="SR14" s="25"/>
+      <c r="SS14" s="25"/>
+      <c r="ST14" s="25"/>
+      <c r="SU14" s="25"/>
+      <c r="SV14" s="25"/>
+      <c r="SW14" s="25"/>
+      <c r="SX14" s="25"/>
+      <c r="SY14" s="25"/>
+      <c r="SZ14" s="25"/>
+      <c r="TA14" s="25"/>
+      <c r="TB14" s="25"/>
+      <c r="TC14" s="25"/>
+      <c r="TD14" s="25"/>
+      <c r="TE14" s="25"/>
+      <c r="TF14" s="25"/>
+      <c r="TG14" s="25"/>
+      <c r="TH14" s="25"/>
+      <c r="TI14" s="25"/>
+      <c r="TJ14" s="25"/>
+      <c r="TK14" s="25"/>
+      <c r="TL14" s="25"/>
+      <c r="TM14" s="25"/>
+      <c r="TN14" s="25"/>
+      <c r="TO14" s="25"/>
+      <c r="TP14" s="25"/>
+      <c r="TQ14" s="25"/>
+      <c r="TR14" s="25"/>
+      <c r="TS14" s="25"/>
+      <c r="TT14" s="25"/>
+      <c r="TU14" s="25"/>
+      <c r="TV14" s="25"/>
+      <c r="TW14" s="25"/>
+      <c r="TX14" s="25"/>
+      <c r="TY14" s="25"/>
+      <c r="TZ14" s="25"/>
+      <c r="UA14" s="25"/>
+      <c r="UB14" s="25"/>
+      <c r="UC14" s="25"/>
+      <c r="UD14" s="25"/>
+      <c r="UE14" s="25"/>
+      <c r="UF14" s="25"/>
+      <c r="UG14" s="25"/>
+      <c r="UH14" s="25"/>
+      <c r="UI14" s="25"/>
+      <c r="UJ14" s="25"/>
+      <c r="UK14" s="25"/>
+      <c r="UL14" s="25"/>
+      <c r="UM14" s="25"/>
+      <c r="UN14" s="25"/>
+      <c r="UO14" s="25"/>
+      <c r="UP14" s="25"/>
+      <c r="UQ14" s="25"/>
+      <c r="UR14" s="25"/>
+      <c r="US14" s="25"/>
+      <c r="UT14" s="25"/>
+      <c r="UU14" s="25"/>
+      <c r="UV14" s="25"/>
+      <c r="UW14" s="25"/>
+      <c r="UX14" s="25"/>
+      <c r="UY14" s="25"/>
+      <c r="UZ14" s="25"/>
+      <c r="VA14" s="25"/>
+      <c r="VB14" s="25"/>
+      <c r="VC14" s="25"/>
+      <c r="VD14" s="25"/>
+      <c r="VE14" s="25"/>
+      <c r="VF14" s="25"/>
+      <c r="VG14" s="25"/>
+      <c r="VH14" s="25"/>
+      <c r="VI14" s="25"/>
+      <c r="VJ14" s="25"/>
+      <c r="VK14" s="25"/>
+      <c r="VL14" s="25"/>
+      <c r="VM14" s="25"/>
+      <c r="VN14" s="25"/>
+      <c r="VO14" s="25"/>
+      <c r="VP14" s="25"/>
+      <c r="VQ14" s="25"/>
+      <c r="VR14" s="25"/>
+      <c r="VS14" s="25"/>
+      <c r="VT14" s="25"/>
+      <c r="VU14" s="25"/>
+      <c r="VV14" s="25"/>
+      <c r="VW14" s="25"/>
+      <c r="VX14" s="25"/>
+      <c r="VY14" s="25"/>
+      <c r="VZ14" s="25"/>
+      <c r="WA14" s="25"/>
+      <c r="WB14" s="25"/>
+      <c r="WC14" s="25"/>
+      <c r="WD14" s="25"/>
+      <c r="WE14" s="25"/>
+      <c r="WF14" s="25"/>
+      <c r="WG14" s="25"/>
+      <c r="WH14" s="25"/>
+      <c r="WI14" s="25"/>
+      <c r="WJ14" s="25"/>
+      <c r="WK14" s="25"/>
+      <c r="WL14" s="25"/>
+      <c r="WM14" s="25"/>
+      <c r="WN14" s="25"/>
+      <c r="WO14" s="25"/>
+      <c r="WP14" s="25"/>
+      <c r="WQ14" s="25"/>
+      <c r="WR14" s="25"/>
+      <c r="WS14" s="25"/>
+      <c r="WT14" s="25"/>
+      <c r="WU14" s="25"/>
+      <c r="WV14" s="25"/>
+      <c r="WW14" s="25"/>
+      <c r="WX14" s="25"/>
+      <c r="WY14" s="25"/>
+      <c r="WZ14" s="25"/>
+      <c r="XA14" s="25"/>
+      <c r="XB14" s="25"/>
+      <c r="XC14" s="25"/>
+      <c r="XD14" s="25"/>
+      <c r="XE14" s="25"/>
+      <c r="XF14" s="25"/>
+      <c r="XG14" s="25"/>
+      <c r="XH14" s="25"/>
+      <c r="XI14" s="25"/>
+      <c r="XJ14" s="25"/>
+      <c r="XK14" s="25"/>
+      <c r="XL14" s="25"/>
+      <c r="XM14" s="25"/>
+      <c r="XN14" s="25"/>
+      <c r="XO14" s="25"/>
+      <c r="XP14" s="25"/>
+      <c r="XQ14" s="25"/>
+      <c r="XR14" s="25"/>
+      <c r="XS14" s="25"/>
+      <c r="XT14" s="25"/>
+      <c r="XU14" s="25"/>
+      <c r="XV14" s="25"/>
+      <c r="XW14" s="25"/>
+      <c r="XX14" s="25"/>
+      <c r="XY14" s="25"/>
+      <c r="XZ14" s="25"/>
+      <c r="YA14" s="25"/>
+      <c r="YB14" s="25"/>
+      <c r="YC14" s="25"/>
+      <c r="YD14" s="25"/>
+      <c r="YE14" s="25"/>
+      <c r="YF14" s="25"/>
+      <c r="YG14" s="25"/>
+      <c r="YH14" s="25"/>
+      <c r="YI14" s="25"/>
+      <c r="YJ14" s="25"/>
+      <c r="YK14" s="25"/>
+      <c r="YL14" s="25"/>
+      <c r="YM14" s="25"/>
+      <c r="YN14" s="25"/>
+      <c r="YO14" s="25"/>
+      <c r="YP14" s="25"/>
+      <c r="YQ14" s="25"/>
+      <c r="YR14" s="25"/>
+      <c r="YS14" s="25"/>
+      <c r="YT14" s="25"/>
+      <c r="YU14" s="25"/>
+      <c r="YV14" s="25"/>
+      <c r="YW14" s="25"/>
+      <c r="YX14" s="25"/>
+      <c r="YY14" s="25"/>
+      <c r="YZ14" s="25"/>
+      <c r="ZA14" s="25"/>
+      <c r="ZB14" s="25"/>
+      <c r="ZC14" s="25"/>
+      <c r="ZD14" s="25"/>
+      <c r="ZE14" s="25"/>
+      <c r="ZF14" s="25"/>
+      <c r="ZG14" s="25"/>
+      <c r="ZH14" s="25"/>
+      <c r="ZI14" s="25"/>
+      <c r="ZJ14" s="25"/>
+      <c r="ZK14" s="25"/>
+      <c r="ZL14" s="25"/>
+      <c r="ZM14" s="25"/>
+      <c r="ZN14" s="25"/>
+      <c r="ZO14" s="25"/>
+      <c r="ZP14" s="25"/>
+      <c r="ZQ14" s="25"/>
+      <c r="ZR14" s="25"/>
+      <c r="ZS14" s="25"/>
+      <c r="ZT14" s="25"/>
+      <c r="ZU14" s="25"/>
+      <c r="ZV14" s="25"/>
+      <c r="ZW14" s="25"/>
+      <c r="ZX14" s="25"/>
+      <c r="ZY14" s="25"/>
+      <c r="ZZ14" s="25"/>
+      <c r="AAA14" s="25"/>
+      <c r="AAB14" s="25"/>
+      <c r="AAC14" s="25"/>
+      <c r="AAD14" s="25"/>
+      <c r="AAE14" s="25"/>
+      <c r="AAF14" s="25"/>
+      <c r="AAG14" s="25"/>
+      <c r="AAH14" s="25"/>
+      <c r="AAI14" s="25"/>
+      <c r="AAJ14" s="25"/>
+      <c r="AAK14" s="25"/>
+      <c r="AAL14" s="25"/>
+      <c r="AAM14" s="25"/>
+      <c r="AAN14" s="25"/>
+      <c r="AAO14" s="25"/>
+      <c r="AAP14" s="25"/>
+      <c r="AAQ14" s="25"/>
+      <c r="AAR14" s="25"/>
+      <c r="AAS14" s="25"/>
+      <c r="AAT14" s="25"/>
+      <c r="AAU14" s="25"/>
+      <c r="AAV14" s="25"/>
+      <c r="AAW14" s="25"/>
+      <c r="AAX14" s="25"/>
+      <c r="AAY14" s="25"/>
+      <c r="AAZ14" s="25"/>
+      <c r="ABA14" s="25"/>
+      <c r="ABB14" s="25"/>
+      <c r="ABC14" s="25"/>
+      <c r="ABD14" s="25"/>
+      <c r="ABE14" s="25"/>
+      <c r="ABF14" s="25"/>
+      <c r="ABG14" s="25"/>
+      <c r="ABH14" s="25"/>
+      <c r="ABI14" s="25"/>
+      <c r="ABJ14" s="25"/>
+      <c r="ABK14" s="25"/>
+      <c r="ABL14" s="25"/>
+      <c r="ABM14" s="25"/>
+      <c r="ABN14" s="25"/>
+      <c r="ABO14" s="25"/>
+      <c r="ABP14" s="25"/>
+      <c r="ABQ14" s="25"/>
+      <c r="ABR14" s="25"/>
+      <c r="ABS14" s="25"/>
+      <c r="ABT14" s="25"/>
+      <c r="ABU14" s="25"/>
+      <c r="ABV14" s="25"/>
+      <c r="ABW14" s="25"/>
+      <c r="ABX14" s="25"/>
+      <c r="ABY14" s="25"/>
+      <c r="ABZ14" s="25"/>
+      <c r="ACA14" s="25"/>
+      <c r="ACB14" s="25"/>
+      <c r="ACC14" s="25"/>
+      <c r="ACD14" s="25"/>
+      <c r="ACE14" s="25"/>
+      <c r="ACF14" s="25"/>
+      <c r="ACG14" s="25"/>
+      <c r="ACH14" s="25"/>
+      <c r="ACI14" s="25"/>
+      <c r="ACJ14" s="25"/>
+      <c r="ACK14" s="25"/>
+      <c r="ACL14" s="25"/>
+      <c r="ACM14" s="25"/>
+      <c r="ACN14" s="25"/>
+      <c r="ACO14" s="25"/>
+      <c r="ACP14" s="25"/>
+      <c r="ACQ14" s="25"/>
+      <c r="ACR14" s="25"/>
+      <c r="ACS14" s="25"/>
+      <c r="ACT14" s="25"/>
+      <c r="ACU14" s="25"/>
+      <c r="ACV14" s="25"/>
+      <c r="ACW14" s="25"/>
+      <c r="ACX14" s="25"/>
+      <c r="ACY14" s="25"/>
+      <c r="ACZ14" s="25"/>
+      <c r="ADA14" s="25"/>
+      <c r="ADB14" s="25"/>
+      <c r="ADC14" s="25"/>
+      <c r="ADD14" s="25"/>
+      <c r="ADE14" s="25"/>
+      <c r="ADF14" s="25"/>
+      <c r="ADG14" s="25"/>
+      <c r="ADH14" s="25"/>
+      <c r="ADI14" s="25"/>
+      <c r="ADJ14" s="25"/>
+      <c r="ADK14" s="25"/>
+      <c r="ADL14" s="25"/>
+      <c r="ADM14" s="25"/>
+      <c r="ADN14" s="25"/>
+      <c r="ADO14" s="25"/>
+      <c r="ADP14" s="25"/>
+      <c r="ADQ14" s="25"/>
+      <c r="ADR14" s="25"/>
+      <c r="ADS14" s="25"/>
+      <c r="ADT14" s="25"/>
+      <c r="ADU14" s="25"/>
+      <c r="ADV14" s="25"/>
+      <c r="ADW14" s="25"/>
+      <c r="ADX14" s="25"/>
+      <c r="ADY14" s="25"/>
+      <c r="ADZ14" s="25"/>
+      <c r="AEA14" s="25"/>
+      <c r="AEB14" s="25"/>
+      <c r="AEC14" s="25"/>
+      <c r="AED14" s="25"/>
+      <c r="AEE14" s="25"/>
+      <c r="AEF14" s="25"/>
+      <c r="AEG14" s="25"/>
+      <c r="AEH14" s="25"/>
+      <c r="AEI14" s="25"/>
+      <c r="AEJ14" s="25"/>
+      <c r="AEK14" s="25"/>
+      <c r="AEL14" s="25"/>
+      <c r="AEM14" s="25"/>
+      <c r="AEN14" s="25"/>
+      <c r="AEO14" s="25"/>
+      <c r="AEP14" s="25"/>
+      <c r="AEQ14" s="25"/>
+      <c r="AER14" s="25"/>
+      <c r="AES14" s="25"/>
+      <c r="AET14" s="25"/>
+      <c r="AEU14" s="25"/>
+      <c r="AEV14" s="25"/>
+      <c r="AEW14" s="25"/>
+      <c r="AEX14" s="25"/>
+      <c r="AEY14" s="25"/>
+      <c r="AEZ14" s="25"/>
+      <c r="AFA14" s="25"/>
+      <c r="AFB14" s="25"/>
+      <c r="AFC14" s="25"/>
+      <c r="AFD14" s="25"/>
+      <c r="AFE14" s="25"/>
+      <c r="AFF14" s="25"/>
+      <c r="AFG14" s="25"/>
+      <c r="AFH14" s="25"/>
+      <c r="AFI14" s="25"/>
+      <c r="AFJ14" s="25"/>
+      <c r="AFK14" s="25"/>
+      <c r="AFL14" s="25"/>
+      <c r="AFM14" s="25"/>
+      <c r="AFN14" s="25"/>
+      <c r="AFO14" s="25"/>
+      <c r="AFP14" s="25"/>
+      <c r="AFQ14" s="25"/>
+      <c r="AFR14" s="25"/>
+      <c r="AFS14" s="25"/>
+      <c r="AFT14" s="25"/>
+      <c r="AFU14" s="25"/>
+      <c r="AFV14" s="25"/>
+      <c r="AFW14" s="25"/>
+      <c r="AFX14" s="25"/>
+      <c r="AFY14" s="25"/>
+      <c r="AFZ14" s="25"/>
+      <c r="AGA14" s="25"/>
+      <c r="AGB14" s="25"/>
+      <c r="AGC14" s="25"/>
+      <c r="AGD14" s="25"/>
+      <c r="AGE14" s="25"/>
+      <c r="AGF14" s="25"/>
+      <c r="AGG14" s="25"/>
+      <c r="AGH14" s="25"/>
+      <c r="AGI14" s="25"/>
+      <c r="AGJ14" s="25"/>
+      <c r="AGK14" s="25"/>
+      <c r="AGL14" s="25"/>
+      <c r="AGM14" s="25"/>
+      <c r="AGN14" s="25"/>
+      <c r="AGO14" s="25"/>
+      <c r="AGP14" s="25"/>
+      <c r="AGQ14" s="25"/>
+      <c r="AGR14" s="25"/>
+      <c r="AGS14" s="25"/>
+      <c r="AGT14" s="25"/>
+      <c r="AGU14" s="25"/>
+      <c r="AGV14" s="25"/>
+      <c r="AGW14" s="25"/>
+      <c r="AGX14" s="25"/>
+      <c r="AGY14" s="25"/>
+      <c r="AGZ14" s="25"/>
+      <c r="AHA14" s="25"/>
+      <c r="AHB14" s="25"/>
+      <c r="AHC14" s="25"/>
+      <c r="AHD14" s="25"/>
+      <c r="AHE14" s="25"/>
+      <c r="AHF14" s="25"/>
+      <c r="AHG14" s="25"/>
+      <c r="AHH14" s="25"/>
+      <c r="AHI14" s="25"/>
+      <c r="AHJ14" s="25"/>
+      <c r="AHK14" s="25"/>
+      <c r="AHL14" s="25"/>
+      <c r="AHM14" s="25"/>
+      <c r="AHN14" s="25"/>
+      <c r="AHO14" s="25"/>
+      <c r="AHP14" s="25"/>
+      <c r="AHQ14" s="25"/>
+      <c r="AHR14" s="25"/>
+      <c r="AHS14" s="25"/>
+      <c r="AHT14" s="25"/>
+      <c r="AHU14" s="25"/>
+      <c r="AHV14" s="25"/>
+      <c r="AHW14" s="25"/>
+      <c r="AHX14" s="25"/>
+      <c r="AHY14" s="25"/>
+      <c r="AHZ14" s="25"/>
+      <c r="AIA14" s="25"/>
+      <c r="AIB14" s="25"/>
+      <c r="AIC14" s="25"/>
+      <c r="AID14" s="25"/>
+      <c r="AIE14" s="25"/>
+      <c r="AIF14" s="25"/>
+      <c r="AIG14" s="25"/>
+      <c r="AIH14" s="25"/>
+      <c r="AII14" s="25"/>
+      <c r="AIJ14" s="25"/>
+      <c r="AIK14" s="25"/>
+      <c r="AIL14" s="25"/>
+      <c r="AIM14" s="25"/>
+      <c r="AIN14" s="25"/>
+      <c r="AIO14" s="25"/>
+      <c r="AIP14" s="25"/>
+      <c r="AIQ14" s="25"/>
+      <c r="AIR14" s="25"/>
+      <c r="AIS14" s="25"/>
+      <c r="AIT14" s="25"/>
+      <c r="AIU14" s="25"/>
+      <c r="AIV14" s="25"/>
+      <c r="AIW14" s="25"/>
+      <c r="AIX14" s="25"/>
+      <c r="AIY14" s="25"/>
+      <c r="AIZ14" s="25"/>
+      <c r="AJA14" s="25"/>
+      <c r="AJB14" s="25"/>
+      <c r="AJC14" s="25"/>
+      <c r="AJD14" s="25"/>
+      <c r="AJE14" s="25"/>
+      <c r="AJF14" s="25"/>
+      <c r="AJG14" s="25"/>
+      <c r="AJH14" s="25"/>
+      <c r="AJI14" s="25"/>
+      <c r="AJJ14" s="25"/>
+      <c r="AJK14" s="25"/>
+      <c r="AJL14" s="25"/>
+      <c r="AJM14" s="25"/>
+      <c r="AJN14" s="25"/>
+      <c r="AJO14" s="25"/>
+      <c r="AJP14" s="25"/>
+      <c r="AJQ14" s="25"/>
+      <c r="AJR14" s="25"/>
+      <c r="AJS14" s="25"/>
+      <c r="AJT14" s="25"/>
+      <c r="AJU14" s="25"/>
+      <c r="AJV14" s="25"/>
+      <c r="AJW14" s="25"/>
+      <c r="AJX14" s="25"/>
+      <c r="AJY14" s="25"/>
+      <c r="AJZ14" s="25"/>
+      <c r="AKA14" s="25"/>
+      <c r="AKB14" s="25"/>
+      <c r="AKC14" s="25"/>
+      <c r="AKD14" s="25"/>
+      <c r="AKE14" s="25"/>
+      <c r="AKF14" s="25"/>
+      <c r="AKG14" s="25"/>
+      <c r="AKH14" s="25"/>
+      <c r="AKI14" s="25"/>
+      <c r="AKJ14" s="25"/>
+      <c r="AKK14" s="25"/>
+      <c r="AKL14" s="25"/>
+      <c r="AKM14" s="25"/>
+      <c r="AKN14" s="25"/>
+      <c r="AKO14" s="25"/>
+      <c r="AKP14" s="25"/>
+      <c r="AKQ14" s="25"/>
+      <c r="AKR14" s="25"/>
+      <c r="AKS14" s="25"/>
+      <c r="AKT14" s="25"/>
+      <c r="AKU14" s="25"/>
+      <c r="AKV14" s="25"/>
+      <c r="AKW14" s="25"/>
+      <c r="AKX14" s="25"/>
+      <c r="AKY14" s="25"/>
+      <c r="AKZ14" s="25"/>
+      <c r="ALA14" s="25"/>
+      <c r="ALB14" s="25"/>
+      <c r="ALC14" s="25"/>
+      <c r="ALD14" s="25"/>
+      <c r="ALE14" s="25"/>
+      <c r="ALF14" s="25"/>
+      <c r="ALG14" s="25"/>
+      <c r="ALH14" s="25"/>
+      <c r="ALI14" s="25"/>
+      <c r="ALJ14" s="25"/>
+      <c r="ALK14" s="25"/>
+      <c r="ALL14" s="25"/>
+      <c r="ALM14" s="25"/>
+      <c r="ALN14" s="25"/>
+      <c r="ALO14" s="25"/>
+      <c r="ALP14" s="25"/>
+      <c r="ALQ14" s="25"/>
+      <c r="ALR14" s="25"/>
+      <c r="ALS14" s="25"/>
+      <c r="ALT14" s="25"/>
+      <c r="ALU14" s="25"/>
+      <c r="ALV14" s="25"/>
+      <c r="ALW14" s="25"/>
+      <c r="ALX14" s="25"/>
+      <c r="ALY14" s="25"/>
+      <c r="ALZ14" s="25"/>
+      <c r="AMA14" s="25"/>
+      <c r="AMB14" s="25"/>
+      <c r="AMC14" s="25"/>
+      <c r="AMD14" s="25"/>
+      <c r="AME14" s="25"/>
+      <c r="AMF14" s="25"/>
+      <c r="AMG14" s="25"/>
+      <c r="AMH14" s="25"/>
+      <c r="AMI14" s="25"/>
+      <c r="AMJ14" s="25"/>
+    </row>
+    <row r="15" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1428,20 +4520,20 @@
       <c r="E15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="5">
         <v>42286</v>
       </c>
       <c r="H15" s="6">
         <v>0</v>
       </c>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1450,20 +4542,20 @@
       <c r="E16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="5">
         <v>42286</v>
       </c>
       <c r="H16" s="6">
         <v>0</v>
       </c>
-      <c r="I16" s="12"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1472,20 +4564,20 @@
       <c r="E17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="5">
         <v>42286</v>
       </c>
       <c r="H17" s="6">
         <v>0</v>
       </c>
-      <c r="I17" s="12"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1494,20 +4586,20 @@
       <c r="E18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="5">
         <v>42286</v>
       </c>
       <c r="H18" s="6">
         <v>0</v>
       </c>
-      <c r="I18" s="12"/>
+      <c r="I18" s="11"/>
     </row>
     <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1516,280 +4608,280 @@
       <c r="E19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="21"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="5">
         <v>42286</v>
       </c>
       <c r="H19" s="6">
         <v>0</v>
       </c>
-      <c r="I19" s="12"/>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="21"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="5">
         <v>42286</v>
       </c>
       <c r="H20" s="6">
         <v>0</v>
       </c>
-      <c r="I20" s="12"/>
+      <c r="I20" s="11"/>
     </row>
     <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="13"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="21"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="5">
         <v>42286</v>
       </c>
       <c r="H21" s="6">
         <v>0</v>
       </c>
-      <c r="I21" s="12"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="21"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="5">
         <v>42286</v>
       </c>
       <c r="H22" s="6">
         <v>0</v>
       </c>
-      <c r="I22" s="12"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="21"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="5">
         <v>42286</v>
       </c>
       <c r="H23" s="6">
         <v>0</v>
       </c>
-      <c r="I23" s="12"/>
+      <c r="I23" s="11"/>
     </row>
     <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="13"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="21"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="5">
         <v>42286</v>
       </c>
       <c r="H24" s="6">
         <v>0</v>
       </c>
-      <c r="I24" s="12"/>
+      <c r="I24" s="11"/>
     </row>
     <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="21"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="5">
         <v>42286</v>
       </c>
       <c r="H25" s="6">
         <v>0</v>
       </c>
-      <c r="I25" s="12"/>
+      <c r="I25" s="11"/>
     </row>
     <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="21"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="5">
         <v>42286</v>
       </c>
       <c r="H26" s="6">
         <v>0</v>
       </c>
-      <c r="I26" s="12"/>
+      <c r="I26" s="11"/>
     </row>
     <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="21"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="5">
         <v>42286</v>
       </c>
       <c r="H27" s="6">
         <v>0</v>
       </c>
-      <c r="I27" s="12"/>
+      <c r="I27" s="11"/>
     </row>
     <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="13"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="5">
         <v>42286</v>
       </c>
       <c r="H28" s="6">
         <v>0</v>
       </c>
-      <c r="I28" s="12"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="13"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="21"/>
+      <c r="F29" s="20"/>
       <c r="G29" s="5">
         <v>42286</v>
       </c>
       <c r="H29" s="6">
         <v>0</v>
       </c>
-      <c r="I29" s="12"/>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="13"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="21"/>
+      <c r="F30" s="20"/>
       <c r="G30" s="5">
         <v>42286</v>
       </c>
       <c r="H30" s="6">
         <v>0</v>
       </c>
-      <c r="I30" s="12"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="13"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="5">
         <v>42286</v>
       </c>
       <c r="H31" s="6">
         <v>0</v>
       </c>
-      <c r="I31" s="12"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="5">
         <v>42286</v>
       </c>
       <c r="H32" s="6">
         <v>0</v>
       </c>
-      <c r="I32" s="12"/>
+      <c r="I32" s="11"/>
     </row>
     <row r="33" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -1798,20 +4890,20 @@
       <c r="E33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="5">
         <v>42286</v>
       </c>
       <c r="H33" s="6">
         <v>0</v>
       </c>
-      <c r="I33" s="12"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -1820,20 +4912,20 @@
       <c r="E34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="5">
         <v>42286</v>
       </c>
       <c r="H34" s="6">
         <v>0</v>
       </c>
-      <c r="I34" s="12"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -1842,20 +4934,20 @@
       <c r="E35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="20"/>
       <c r="G35" s="5">
         <v>42286</v>
       </c>
       <c r="H35" s="6">
         <v>0</v>
       </c>
-      <c r="I35" s="12"/>
+      <c r="I35" s="11"/>
     </row>
     <row r="36" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -1864,20 +4956,20 @@
       <c r="E36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="21"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="5">
         <v>42286</v>
       </c>
       <c r="H36" s="6">
         <v>0</v>
       </c>
-      <c r="I36" s="12"/>
+      <c r="I36" s="11"/>
     </row>
     <row r="37" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -1886,22 +4978,22 @@
       <c r="E37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="21"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="5">
         <v>42286</v>
       </c>
       <c r="H37" s="6">
         <v>0</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I37" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -1910,7 +5002,7 @@
       <c r="E38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="21">
+      <c r="F38" s="20">
         <v>42284</v>
       </c>
       <c r="G38" s="5">
@@ -1919,13 +5011,13 @@
       <c r="H38" s="6">
         <v>1</v>
       </c>
-      <c r="I38" s="12"/>
+      <c r="I38" s="11"/>
     </row>
     <row r="39" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -1934,7 +5026,7 @@
       <c r="E39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="21">
+      <c r="F39" s="20">
         <v>42284</v>
       </c>
       <c r="G39" s="5">
@@ -1943,13 +5035,13 @@
       <c r="H39" s="6">
         <v>1</v>
       </c>
-      <c r="I39" s="12"/>
+      <c r="I39" s="11"/>
     </row>
     <row r="40" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -1958,7 +5050,7 @@
       <c r="E40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="21">
+      <c r="F40" s="20">
         <v>42284</v>
       </c>
       <c r="G40" s="5">
@@ -1967,62 +5059,62 @@
       <c r="H40" s="6">
         <v>1</v>
       </c>
-      <c r="I40" s="12"/>
+      <c r="I40" s="11"/>
     </row>
     <row r="41" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="13"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="21"/>
+      <c r="F41" s="20"/>
       <c r="G41" s="5">
         <v>42286</v>
       </c>
       <c r="H41" s="6">
         <v>0</v>
       </c>
-      <c r="I41" s="12"/>
+      <c r="I41" s="11"/>
     </row>
     <row r="42" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="13"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="21"/>
+      <c r="F42" s="20"/>
       <c r="G42" s="5">
         <v>42286</v>
       </c>
       <c r="H42" s="6">
         <v>0</v>
       </c>
-      <c r="I42" s="12"/>
+      <c r="I42" s="11"/>
     </row>
     <row r="43" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="21">
+      <c r="F43" s="20">
         <v>42282</v>
       </c>
       <c r="G43" s="5">
@@ -2031,42 +5123,42 @@
       <c r="H43" s="6">
         <v>1</v>
       </c>
-      <c r="I43" s="12"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="21"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="20"/>
       <c r="G44" s="5">
         <v>42288</v>
       </c>
       <c r="H44" s="6">
         <v>0</v>
       </c>
-      <c r="I44" s="12"/>
+      <c r="I44" s="11"/>
     </row>
     <row r="45" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F45" s="21">
+      <c r="F45" s="20">
         <v>42282</v>
       </c>
       <c r="G45" s="5">
@@ -2075,31 +5167,31 @@
       <c r="H45" s="6">
         <v>1</v>
       </c>
-      <c r="I45" s="12" t="s">
+      <c r="I45" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="46" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="21"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="20"/>
       <c r="G46" s="5">
         <v>42286</v>
       </c>
-      <c r="H46" s="14"/>
-      <c r="I46" s="12"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="11"/>
     </row>
     <row r="47" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -2108,15 +5200,15 @@
       <c r="E47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="21"/>
+      <c r="F47" s="20"/>
       <c r="G47" s="5">
         <v>42286</v>
       </c>
-      <c r="H47" s="14"/>
-      <c r="I47" s="12"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="11"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+g/uNa6hwgd3qQkJ7Pwi7DSrUm70jAwsYBWXjBvFzLsGuEKn8SILdmJApe0lNh/jAqorM7svFeytstLmq95Tkg==" saltValue="2XoZm9EUZNjCwsapgNRmIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dlVqSI3/zTpv3cn916vFPH+NHY1lHwB99o+0/aaxyQP50BzJtTj3mRer5hUmMb5tUZz8u8Z/OBQxuqqAmKUmYQ==" saltValue="CdleC3s2rMMn0xTwtJ6Ouw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="H12">
     <cfRule type="dataBar" priority="3">
       <dataBar>
@@ -2426,7 +5518,7 @@
       <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2482,79 +5574,79 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>1</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="18">
+      <c r="B15" s="17">
         <v>2</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>3</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <v>4</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="19" spans="2:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Elais and Anson are done. Typo fixes
</commit_message>
<xml_diff>
--- a/docs/Tasks List.xlsx
+++ b/docs/Tasks List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salim_000\Documents\GitHub\TradingApp\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\GitHub\TradingApp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="78">
   <si>
     <t>Task</t>
   </si>
@@ -136,27 +136,6 @@
     <t>Aaron</t>
   </si>
   <si>
-    <t>US03.03.01</t>
-  </si>
-  <si>
-    <t>US03.04.01</t>
-  </si>
-  <si>
-    <t>US03.05.01</t>
-  </si>
-  <si>
-    <t>US03.06.01</t>
-  </si>
-  <si>
-    <t>US03.07.01</t>
-  </si>
-  <si>
-    <t>US03.08.01</t>
-  </si>
-  <si>
-    <t>US03.09.01</t>
-  </si>
-  <si>
     <t>US06.01.01</t>
   </si>
   <si>
@@ -251,6 +230,36 @@
   </si>
   <si>
     <t>I  uploaded to github</t>
+  </si>
+  <si>
+    <t>US04.01.01</t>
+  </si>
+  <si>
+    <t>US04.02.01</t>
+  </si>
+  <si>
+    <t>US04.03.01</t>
+  </si>
+  <si>
+    <t>US04.04.01</t>
+  </si>
+  <si>
+    <t>US04.05.01</t>
+  </si>
+  <si>
+    <t>US04.06.01</t>
+  </si>
+  <si>
+    <t>US04.07.01</t>
+  </si>
+  <si>
+    <t>US04.08.01</t>
+  </si>
+  <si>
+    <t>US04.09.01</t>
+  </si>
+  <si>
+    <t>US10.02.01</t>
   </si>
 </sst>
 </file>
@@ -380,18 +389,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -469,9 +469,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,6 +486,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -586,8 +592,8 @@
       <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>454261</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1061640</xdr:rowOff>
     </xdr:to>
@@ -1146,19 +1152,22 @@
   </sheetPr>
   <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="4"/>
-    <col min="3" max="3" width="8.85546875" style="5"/>
-    <col min="4" max="5" width="8.85546875" style="4"/>
-    <col min="6" max="6" width="8.85546875" style="6"/>
-    <col min="7" max="8" width="8.85546875" style="4"/>
-    <col min="9" max="9" width="8.85546875" style="5"/>
-    <col min="10" max="1025" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="28.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.81640625" style="2"/>
+    <col min="10" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1167,7 +1176,7 @@
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1" s="7"/>
+      <c r="F1" s="4"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -2193,7 +2202,7 @@
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2" s="7"/>
+      <c r="F2" s="4"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -3219,7 +3228,7 @@
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="4"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
@@ -4241,28 +4250,28 @@
     </row>
     <row r="4" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J4"/>
@@ -5283,28 +5292,28 @@
     </row>
     <row r="5" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>42282</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>42286</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="9">
         <v>1</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="6"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -6323,28 +6332,28 @@
     </row>
     <row r="6" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>42282</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>42286</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>1</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="6"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -7363,28 +7372,28 @@
     </row>
     <row r="7" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>42282</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>42286</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="9">
         <v>1</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="6"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -8403,28 +8412,28 @@
     </row>
     <row r="8" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>42282</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>42286</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <v>1</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="6"/>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -9441,78 +9450,78 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="1:1024" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17">
+      <c r="F9" s="13"/>
+      <c r="G9" s="14">
         <v>42286</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
         <v>0</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1024" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
+    <row r="10" spans="1:1024" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="17">
+      <c r="F10" s="18"/>
+      <c r="G10" s="14">
         <v>42286</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="15">
         <v>0</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>42282</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>42286</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="9">
         <v>1</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="21"/>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
@@ -10531,28 +10540,28 @@
     </row>
     <row r="12" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>42282</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="8">
         <v>42286</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="9">
         <v>1</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="21"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -11571,28 +11580,28 @@
     </row>
     <row r="13" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>42282</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <v>42286</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="9">
         <v>1</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="21"/>
       <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
@@ -12609,768 +12618,806 @@
       <c r="AMI13"/>
       <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1024" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+    <row r="14" spans="1:1024" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="17">
+      <c r="F14" s="18"/>
+      <c r="G14" s="14">
         <v>42286</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="15">
         <v>0</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="11">
+      <c r="F15" s="23"/>
+      <c r="G15" s="8">
         <v>42286</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="9">
         <v>0</v>
       </c>
-      <c r="I15" s="24" t="s">
-        <v>74</v>
+      <c r="I15" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:1024" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="11">
+      <c r="F16" s="23"/>
+      <c r="G16" s="8">
         <v>42286</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="9">
         <v>0</v>
       </c>
-      <c r="I16" s="24" t="s">
-        <v>74</v>
+      <c r="I16" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="11">
+      <c r="F17" s="23"/>
+      <c r="G17" s="8">
         <v>42286</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="9">
         <v>0</v>
       </c>
-      <c r="I17" s="24" t="s">
-        <v>74</v>
+      <c r="I17" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="11">
+      <c r="F18" s="23"/>
+      <c r="G18" s="8">
         <v>42286</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="9">
         <v>0</v>
       </c>
-      <c r="I18" s="24" t="s">
-        <v>74</v>
+      <c r="I18" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="11">
+      <c r="F19" s="23"/>
+      <c r="G19" s="8">
         <v>42286</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="9">
         <v>0</v>
       </c>
-      <c r="I19" s="24" t="s">
-        <v>74</v>
+      <c r="I19" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0</v>
-      </c>
-      <c r="I20" s="24"/>
+      <c r="E20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G20" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H21" s="12">
-        <v>0</v>
-      </c>
-      <c r="I21" s="24"/>
+      <c r="E21" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G21" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H22" s="12">
-        <v>0</v>
-      </c>
-      <c r="I22" s="24"/>
+      <c r="E22" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G22" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
+      <c r="I22" s="21"/>
     </row>
     <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H23" s="12">
-        <v>0</v>
-      </c>
-      <c r="I23" s="24"/>
+      <c r="E23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G23" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H23" s="9">
+        <v>1</v>
+      </c>
+      <c r="I23" s="21"/>
     </row>
     <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="25" t="s">
+      <c r="B24" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="11">
+      <c r="F24" s="23"/>
+      <c r="G24" s="8">
         <v>42286</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="9">
         <v>0</v>
       </c>
-      <c r="I24" s="24"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="25" t="s">
+      <c r="B25" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="11">
+      <c r="F25" s="23"/>
+      <c r="G25" s="8">
         <v>42286</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="9">
         <v>0</v>
       </c>
-      <c r="I25" s="24"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="25" t="s">
+      <c r="B26" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="11">
+      <c r="F26" s="23"/>
+      <c r="G26" s="8">
         <v>42286</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="9">
         <v>0</v>
       </c>
-      <c r="I26" s="24"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="25" t="s">
+      <c r="B27" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="11">
+      <c r="F27" s="23"/>
+      <c r="G27" s="8">
         <v>42286</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="9">
         <v>0</v>
       </c>
-      <c r="I27" s="24"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="25" t="s">
+      <c r="B28" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="26"/>
-      <c r="G28" s="11">
+      <c r="F28" s="23"/>
+      <c r="G28" s="8">
         <v>42286</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="9">
         <v>0</v>
       </c>
-      <c r="I28" s="24"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="11">
+      <c r="F29" s="23"/>
+      <c r="G29" s="8">
         <v>42286</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="9">
         <v>0</v>
       </c>
-      <c r="I29" s="24"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="25" t="s">
+      <c r="B30" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="11">
+      <c r="F30" s="23"/>
+      <c r="G30" s="8">
         <v>42286</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="9">
         <v>0</v>
       </c>
-      <c r="I30" s="24"/>
+      <c r="I30" s="21"/>
     </row>
     <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="25" t="s">
+      <c r="B31" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="11">
+      <c r="F31" s="23"/>
+      <c r="G31" s="8">
         <v>42286</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="9">
         <v>0</v>
       </c>
-      <c r="I31" s="24"/>
+      <c r="I31" s="21"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="25" t="s">
+      <c r="B32" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="11">
+      <c r="F32" s="23"/>
+      <c r="G32" s="8">
         <v>42286</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="9">
         <v>0</v>
       </c>
-      <c r="I32" s="24"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="25" t="s">
+      <c r="B33" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H33" s="12">
-        <v>0</v>
-      </c>
-      <c r="I33" s="24"/>
+      <c r="E33" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G33" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H33" s="9">
+        <v>1</v>
+      </c>
+      <c r="I33" s="21"/>
     </row>
     <row r="34" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="25" t="s">
+      <c r="B34" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H34" s="12">
-        <v>0</v>
-      </c>
-      <c r="I34" s="24"/>
+      <c r="E34" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G34" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H34" s="9">
+        <v>1</v>
+      </c>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="25" t="s">
+      <c r="B35" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H35" s="12">
-        <v>0</v>
-      </c>
-      <c r="I35" s="24"/>
+      <c r="E35" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G35" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H35" s="9">
+        <v>1</v>
+      </c>
+      <c r="I35" s="21"/>
     </row>
     <row r="36" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="25" t="s">
+      <c r="B36" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="26"/>
-      <c r="G36" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H36" s="12">
-        <v>0</v>
-      </c>
-      <c r="I36" s="24"/>
+      <c r="E36" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G36" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H36" s="9">
+        <v>1</v>
+      </c>
+      <c r="I36" s="21"/>
     </row>
     <row r="37" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="25" t="s">
+      <c r="B37" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="26"/>
-      <c r="G37" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H37" s="12">
-        <v>0</v>
-      </c>
-      <c r="I37" s="24" t="s">
-        <v>48</v>
+      <c r="E37" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G37" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H37" s="9">
+        <v>1</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="8" t="s">
+      <c r="B38" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="23">
         <v>42284</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="8">
         <v>42286</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H38" s="9">
         <v>1</v>
       </c>
-      <c r="I38" s="24"/>
+      <c r="I38" s="21"/>
     </row>
     <row r="39" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="8" t="s">
+      <c r="B39" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F39" s="23">
         <v>42284</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="8">
         <v>42286</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="9">
         <v>1</v>
       </c>
-      <c r="I39" s="24"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="B40" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="26">
+      <c r="F40" s="23">
         <v>42284</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="8">
         <v>42286</v>
       </c>
-      <c r="H40" s="12">
+      <c r="H40" s="9">
         <v>1</v>
       </c>
-      <c r="I40" s="24"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="8" t="s">
+      <c r="B41" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="26"/>
-      <c r="G41" s="11">
+      <c r="F41" s="23"/>
+      <c r="G41" s="8">
         <v>42286</v>
       </c>
-      <c r="H41" s="12">
+      <c r="H41" s="9">
         <v>0</v>
       </c>
-      <c r="I41" s="24"/>
+      <c r="I41" s="21"/>
     </row>
     <row r="42" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="8" t="s">
+      <c r="B42" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="26"/>
-      <c r="G42" s="11">
+      <c r="F42" s="23"/>
+      <c r="G42" s="8">
         <v>42286</v>
       </c>
-      <c r="H42" s="12">
+      <c r="H42" s="9">
         <v>0</v>
       </c>
-      <c r="I42" s="24"/>
+      <c r="I42" s="21"/>
     </row>
     <row r="43" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="25" t="s">
+      <c r="B43" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="23" t="s">
+      <c r="E43" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="26">
+      <c r="F43" s="23">
         <v>42282</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="8">
         <v>42287</v>
       </c>
-      <c r="H43" s="12">
+      <c r="H43" s="9">
         <v>1</v>
       </c>
-      <c r="I43" s="24"/>
+      <c r="I43" s="21"/>
     </row>
     <row r="44" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="25" t="s">
+      <c r="B44" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="11">
-        <v>42288</v>
-      </c>
-      <c r="H44" s="12">
-        <v>0</v>
-      </c>
-      <c r="I44" s="24"/>
+      <c r="E44" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G44" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="21"/>
     </row>
     <row r="45" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="25" t="s">
+      <c r="B45" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="23" t="s">
+      <c r="E45" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="26">
+      <c r="F45" s="23">
         <v>42282</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G45" s="8">
         <v>42289</v>
       </c>
-      <c r="H45" s="12">
+      <c r="H45" s="9">
         <v>1</v>
       </c>
-      <c r="I45" s="24" t="s">
-        <v>57</v>
+      <c r="I45" s="21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="25" t="s">
+      <c r="B46" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H46" s="27"/>
-      <c r="I46" s="24"/>
+      <c r="D46" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G46" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="21"/>
     </row>
     <row r="47" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="25" t="s">
+      <c r="B47" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="26"/>
-      <c r="G47" s="11">
-        <v>42286</v>
-      </c>
-      <c r="H47" s="27"/>
-      <c r="I47" s="24"/>
+      <c r="E47" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="23">
+        <v>42282</v>
+      </c>
+      <c r="G47" s="8">
+        <v>42287</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1</v>
+      </c>
+      <c r="I47" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TgtgIJQzy+Es/eiXfRZad1kL9I0lBNTh4slXrFLI2uf8iSp60aYZJ+mAgIv63nBc85B8jO8+5GskmwZRbHvIKA==" saltValue="EcowE1tKUOQtKZwc8bg6Kg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="H12">
     <cfRule type="dataBar" priority="2">
       <dataBar>
@@ -13495,9 +13542,9 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.85546875" style="4"/>
+    <col min="1" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13534,163 +13581,163 @@
       <c r="J3"/>
     </row>
     <row r="4" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8">
         <v>42296</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="9">
         <v>0</v>
       </c>
-      <c r="I5" s="28" t="e">
+      <c r="I5" s="24" t="e">
         <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#REF!</v>
       </c>
-      <c r="J5" s="8"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
         <v>42303</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>0</v>
       </c>
-      <c r="I6" s="28" t="e">
+      <c r="I6" s="24" t="e">
         <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="8"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="11">
+      <c r="F7" s="25"/>
+      <c r="G7" s="8">
         <v>42330</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="9">
         <v>0</v>
       </c>
-      <c r="I7" s="28" t="e">
+      <c r="I7" s="24" t="e">
         <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#REF!</v>
       </c>
-      <c r="J7" s="8"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8">
         <v>42324</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <v>0</v>
       </c>
-      <c r="I8" s="28" t="e">
+      <c r="I8" s="24" t="e">
         <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#REF!</v>
       </c>
-      <c r="J8" s="8"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="11">
+      <c r="F9" s="25"/>
+      <c r="G9" s="8">
         <v>42338</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="9">
         <v>0</v>
       </c>
-      <c r="I9" s="28" t="e">
+      <c r="I9" s="24" t="e">
         <f ca="1">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#REF!</v>
       </c>
-      <c r="J9" s="8"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10"/>
@@ -13726,79 +13773,79 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="B13" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
     </row>
     <row r="14" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="32">
+      <c r="B14" s="28">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="C14" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
     </row>
     <row r="15" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="33">
+      <c r="B15" s="29">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="C15" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="32">
+      <c r="B16" s="28">
         <v>3</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="C16" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
     </row>
     <row r="17" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="33">
+      <c r="B17" s="29">
         <v>4</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="C17" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="19" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -13881,9 +13928,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.85546875"/>
+    <col min="1" max="1025" width="8.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -13898,7 +13945,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -13918,7 +13965,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated task list, we are done for project part 2
</commit_message>
<xml_diff>
--- a/docs/Tasks List.xlsx
+++ b/docs/Tasks List.xlsx
@@ -17,7 +17,9 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Milestones!$4:$4</definedName>
     <definedName function="false" hidden="false" name="Team_Members" vbProcedure="false">Sheet2!$A$1:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Hand-In 2'!$4:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Hand-In 2'!$4:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Milestones!$4:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">Milestones!$4:$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -59,7 +61,7 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>Not Started</t>
+    <t>Complete</t>
   </si>
   <si>
     <t>Storyboard</t>
@@ -72,9 +74,6 @@
   </si>
   <si>
     <t>Joshua</t>
-  </si>
-  <si>
-    <t>Complete</t>
   </si>
   <si>
     <t>US01.02.01</t>
@@ -231,6 +230,9 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
   <si>
     <t>2nd Milestone Complete</t>
@@ -431,7 +433,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -444,32 +446,28 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -477,55 +475,55 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -533,15 +531,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -641,15 +639,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:colOff>108360</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>480960</xdr:colOff>
+      <xdr:colOff>507600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1052280</xdr:rowOff>
+      <xdr:rowOff>1043280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -658,12 +656,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="792000" y="182160"/>
-          <a:ext cx="7722000" cy="1050840"/>
+          <a:off x="819360" y="173160"/>
+          <a:ext cx="9324360" cy="1050840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -713,15 +712,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>198000</xdr:colOff>
+      <xdr:colOff>225000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>170640</xdr:colOff>
+      <xdr:colOff>197280</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>899640</xdr:rowOff>
+      <xdr:rowOff>890640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -730,12 +729,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13311720" y="30240"/>
-          <a:ext cx="684000" cy="1050120"/>
+          <a:off x="19602000" y="21240"/>
+          <a:ext cx="1919160" cy="1050120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -790,15 +790,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:colOff>108000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>111600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1052280</xdr:rowOff>
+      <xdr:rowOff>1042920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -807,12 +807,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="792000" y="182160"/>
-          <a:ext cx="6404760" cy="1050840"/>
+          <a:off x="819000" y="173160"/>
+          <a:ext cx="6404400" cy="1050480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -862,15 +863,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>197640</xdr:colOff>
+      <xdr:colOff>224640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>170640</xdr:colOff>
+      <xdr:colOff>197280</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>899640</xdr:rowOff>
+      <xdr:rowOff>890280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -879,12 +880,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7309440" y="30240"/>
-          <a:ext cx="684360" cy="1050120"/>
+          <a:off x="7336440" y="21240"/>
+          <a:ext cx="684000" cy="1049760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -941,8 +943,8 @@
   </sheetPr>
   <dimension ref="1:47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -951,12 +953,12 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.1741071428571"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="24.6294642857143"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.0892857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.90625"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="21.4598214285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.4598214285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2678571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="8.82142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.82142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="37.78125"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.7276785714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.1428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="24.1428571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.82142857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -965,7 +967,7 @@
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
@@ -1991,7 +1993,7 @@
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
@@ -3017,7 +3019,7 @@
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
@@ -4039,28 +4041,28 @@
     </row>
     <row r="4" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="0"/>
@@ -5081,28 +5083,28 @@
     </row>
     <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>42282</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H5" s="9" t="n">
+      <c r="H5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
       <c r="L5" s="0"/>
@@ -6121,28 +6123,28 @@
     </row>
     <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>42282</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H6" s="9" t="n">
+      <c r="H6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
       <c r="L6" s="0"/>
@@ -7161,28 +7163,28 @@
     </row>
     <row r="7" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="6" t="n">
         <v>42282</v>
       </c>
-      <c r="G7" s="8" t="n">
+      <c r="G7" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H7" s="9" t="n">
+      <c r="H7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
@@ -8201,28 +8203,28 @@
     </row>
     <row r="8" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="7" t="n">
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="n">
         <v>42282</v>
       </c>
-      <c r="G8" s="8" t="n">
+      <c r="G8" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H8" s="9" t="n">
+      <c r="H8" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
@@ -9239,53 +9241,53 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="10" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11" t="s">
+    <row r="9" s="9" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" s="13" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H9" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H9" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="13" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H10" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="14" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H10" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>19</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -10305,28 +10307,28 @@
     </row>
     <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
-      <c r="B11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="7" t="n">
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6" t="n">
         <v>42282</v>
       </c>
-      <c r="G11" s="8" t="n">
+      <c r="G11" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H11" s="9" t="n">
+      <c r="H11" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
@@ -11345,28 +11347,28 @@
     </row>
     <row r="12" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
-      <c r="B12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="n">
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="6" t="n">
         <v>42282</v>
       </c>
-      <c r="G12" s="8" t="n">
+      <c r="G12" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H12" s="9" t="n">
+      <c r="H12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="21"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
       <c r="L12" s="0"/>
@@ -12385,28 +12387,28 @@
     </row>
     <row r="13" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
-      <c r="B13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="7" t="n">
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="6" t="n">
         <v>42282</v>
       </c>
-      <c r="G13" s="8" t="n">
+      <c r="G13" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H13" s="9" t="n">
+      <c r="H13" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="21"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
       <c r="L13" s="0"/>
@@ -13423,835 +13425,835 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="10" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="12" t="s">
+    <row r="14" s="9" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="13" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="14" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H14" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="22" t="n">
+        <v>42285</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H15" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="23" t="n">
-        <v>42285</v>
-      </c>
-      <c r="G15" s="8" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H15" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="22" t="n">
+        <v>42285</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H16" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="23" t="n">
-        <v>42285</v>
-      </c>
-      <c r="G16" s="8" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="22" t="s">
+      <c r="B17" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="22" t="n">
+        <v>42285</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="23" t="n">
-        <v>42285</v>
-      </c>
-      <c r="G17" s="8" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H17" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="22" t="s">
+      <c r="B18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="22" t="n">
+        <v>42285</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H18" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="23" t="n">
-        <v>42285</v>
-      </c>
-      <c r="G18" s="8" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="22" t="n">
+        <v>42285</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="23" t="n">
-        <v>42285</v>
-      </c>
-      <c r="G19" s="8" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H19" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="23" t="n">
+      <c r="E20" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G20" s="8" t="n">
+      <c r="G20" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H20" s="9" t="n">
+      <c r="H20" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="21"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="21" t="s">
+      <c r="B21" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="23" t="n">
+      <c r="E21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G21" s="8" t="n">
+      <c r="G21" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H21" s="9" t="n">
+      <c r="H21" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="21"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="B22" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="23" t="n">
+      <c r="E22" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G22" s="8" t="n">
+      <c r="G22" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H22" s="9" t="n">
+      <c r="H22" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="21"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="B23" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="23" t="n">
+      <c r="E23" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G23" s="8" t="n">
+      <c r="G23" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H23" s="9" t="n">
+      <c r="H23" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="21"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="23" t="n">
+      <c r="E24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="22" t="n">
         <v>42285</v>
       </c>
-      <c r="G24" s="8" t="n">
+      <c r="G24" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H24" s="9" t="n">
+      <c r="H24" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="21"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="22" t="s">
+      <c r="B25" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="23" t="n">
+      <c r="E25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="22" t="n">
         <v>42286</v>
       </c>
-      <c r="G25" s="8" t="n">
+      <c r="G25" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H25" s="9" t="n">
+      <c r="H25" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I25" s="21"/>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="B26" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="23" t="n">
+      <c r="E26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="22" t="n">
         <v>42287</v>
       </c>
-      <c r="G26" s="8" t="n">
+      <c r="G26" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H26" s="9" t="n">
+      <c r="H26" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I26" s="21"/>
+      <c r="I26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="B27" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="23" t="n">
+      <c r="E27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="22" t="n">
         <v>42288</v>
       </c>
-      <c r="G27" s="8" t="n">
+      <c r="G27" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H27" s="9" t="n">
+      <c r="H27" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I27" s="21"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="B28" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="23" t="n">
+      <c r="E28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="22" t="n">
         <v>42289</v>
       </c>
-      <c r="G28" s="8" t="n">
+      <c r="G28" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H28" s="9" t="n">
+      <c r="H28" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="21"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="B29" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="23" t="n">
+      <c r="E29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="22" t="n">
         <v>42290</v>
       </c>
-      <c r="G29" s="8" t="n">
+      <c r="G29" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H29" s="9" t="n">
+      <c r="H29" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I29" s="21"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="B30" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="23" t="n">
+      <c r="E30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="22" t="n">
         <v>42291</v>
       </c>
-      <c r="G30" s="8" t="n">
+      <c r="G30" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H30" s="9" t="n">
+      <c r="H30" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I30" s="21"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="B31" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="23" t="n">
+      <c r="E31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="22" t="n">
         <v>42292</v>
       </c>
-      <c r="G31" s="8" t="n">
+      <c r="G31" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H31" s="9" t="n">
+      <c r="H31" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I31" s="21"/>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="B32" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="23" t="n">
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="22" t="n">
         <v>42293</v>
       </c>
-      <c r="G32" s="8" t="n">
+      <c r="G32" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H32" s="9" t="n">
+      <c r="H32" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="21"/>
+      <c r="I32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="B33" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="23" t="n">
+      <c r="E33" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G33" s="8" t="n">
+      <c r="G33" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H33" s="9" t="n">
+      <c r="H33" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I33" s="21"/>
+      <c r="I33" s="20"/>
     </row>
     <row r="34" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="B34" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="23" t="n">
+      <c r="E34" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G34" s="8" t="n">
+      <c r="G34" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H34" s="9" t="n">
+      <c r="H34" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I34" s="21"/>
+      <c r="I34" s="20"/>
     </row>
     <row r="35" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="B35" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="23" t="n">
+      <c r="E35" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G35" s="8" t="n">
+      <c r="G35" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H35" s="9" t="n">
+      <c r="H35" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I35" s="21"/>
+      <c r="I35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="B36" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="23" t="n">
+      <c r="E36" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G36" s="8" t="n">
+      <c r="G36" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H36" s="9" t="n">
+      <c r="H36" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="21"/>
+      <c r="I36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="22" t="n">
+        <v>42282</v>
+      </c>
+      <c r="G37" s="7" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H37" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="23" t="n">
-        <v>42282</v>
-      </c>
-      <c r="G37" s="8" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H37" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I37" s="21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="23" t="n">
+      <c r="E38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="22" t="n">
         <v>42284</v>
       </c>
-      <c r="G38" s="8" t="n">
+      <c r="G38" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H38" s="9" t="n">
+      <c r="H38" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I38" s="21"/>
+      <c r="I38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="22" t="s">
+      <c r="B39" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="C39" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="23" t="n">
+      <c r="E39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="22" t="n">
         <v>42284</v>
       </c>
-      <c r="G39" s="8" t="n">
+      <c r="G39" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H39" s="9" t="n">
+      <c r="H39" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I39" s="21"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="B40" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="23" t="n">
+      <c r="E40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="22" t="n">
         <v>42284</v>
       </c>
-      <c r="G40" s="8" t="n">
+      <c r="G40" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H40" s="9" t="n">
+      <c r="H40" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I40" s="21"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="22" t="s">
+      <c r="B41" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="23" t="n">
+      <c r="E41" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="22" t="n">
         <v>42285</v>
       </c>
-      <c r="G41" s="8" t="n">
+      <c r="G41" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H41" s="9" t="n">
+      <c r="H41" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I41" s="21"/>
+      <c r="I41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="22" t="s">
+      <c r="B42" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="23" t="n">
+      <c r="E42" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="22" t="n">
         <v>42285</v>
       </c>
-      <c r="G42" s="8" t="n">
+      <c r="G42" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H42" s="9" t="n">
+      <c r="H42" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I42" s="21"/>
+      <c r="I42" s="20"/>
     </row>
     <row r="43" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="23" t="n">
+      <c r="E43" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G43" s="8" t="n">
+      <c r="G43" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H43" s="9" t="n">
+      <c r="H43" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I43" s="21"/>
+      <c r="I43" s="20"/>
     </row>
     <row r="44" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="20" t="s">
+      <c r="B44" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="23" t="n">
+      <c r="E44" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G44" s="8" t="n">
+      <c r="G44" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H44" s="9" t="n">
+      <c r="H44" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I44" s="21"/>
+      <c r="I44" s="20"/>
     </row>
     <row r="45" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="22" t="n">
+        <v>42282</v>
+      </c>
+      <c r="G45" s="7" t="n">
+        <v>42286</v>
+      </c>
+      <c r="H45" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="23" t="n">
-        <v>42282</v>
-      </c>
-      <c r="G45" s="8" t="n">
-        <v>42286</v>
-      </c>
-      <c r="H45" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I45" s="21" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="20" t="s">
+      <c r="B46" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E46" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="23" t="n">
+      <c r="E46" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G46" s="8" t="n">
+      <c r="G46" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H46" s="9" t="n">
+      <c r="H46" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I46" s="21"/>
+      <c r="I46" s="20"/>
     </row>
     <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="B47" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="23" t="n">
+      <c r="E47" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="22" t="n">
         <v>42282</v>
       </c>
-      <c r="G47" s="8" t="n">
+      <c r="G47" s="7" t="n">
         <v>42286</v>
       </c>
-      <c r="H47" s="9" t="n">
+      <c r="H47" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I47" s="21"/>
+      <c r="I47" s="20"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" password="af79" objects="true" scenarios="true"/>
@@ -14264,7 +14266,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{61A19066-59F0-4DE0-94FF-9BD5AF1A1566}</x14:id>
+          <x14:id>{5524F688-20DA-46F3-B0C6-A583C1AFBF1B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -14278,7 +14280,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{39D4B9AA-7A72-4475-A0D5-AA28916D9DBB}</x14:id>
+          <x14:id>{13FBD1E9-B086-488A-A326-6F131D1287A0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -14292,7 +14294,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E0172045-8759-4440-8A7B-30D671D0E5A1}</x14:id>
+          <x14:id>{9B6253E7-EA80-4222-86FC-74A3D081C4A1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -14331,7 +14333,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{61A19066-59F0-4DE0-94FF-9BD5AF1A1566}">
+          <x14:cfRule type="dataBar" id="{5524F688-20DA-46F3-B0C6-A583C1AFBF1B}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic">
               <x14:cfvo type="autoMin" value="0"/>
               <x14:cfvo type="autoMax" value="0"/>
@@ -14342,7 +14344,7 @@
           <xm:sqref>H12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{39D4B9AA-7A72-4475-A0D5-AA28916D9DBB}">
+          <x14:cfRule type="dataBar" id="{13FBD1E9-B086-488A-A326-6F131D1287A0}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic">
               <x14:cfvo type="autoMin" value="0"/>
               <x14:cfvo type="autoMax" value="0"/>
@@ -14353,7 +14355,7 @@
           <xm:sqref>H11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E0172045-8759-4440-8A7B-30D671D0E5A1}">
+          <x14:cfRule type="dataBar" id="{9B6253E7-EA80-4222-86FC-74A3D081C4A1}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic">
               <x14:cfvo type="autoMin" value="0"/>
               <x14:cfvo type="autoMax" value="0"/>
@@ -14419,163 +14421,163 @@
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="I4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="n">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="n">
         <v>42296</v>
       </c>
-      <c r="H5" s="9" t="n">
+      <c r="H5" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="24" t="e">
+      <c r="I5" s="23" t="e">
         <f aca="false">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="n">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="n">
         <v>42303</v>
       </c>
-      <c r="H6" s="9" t="n">
+      <c r="H6" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="24" t="e">
+      <c r="I6" s="23" t="e">
         <f aca="false">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="8" t="n">
+      <c r="F7" s="24"/>
+      <c r="G7" s="7" t="n">
         <v>42330</v>
       </c>
-      <c r="H7" s="9" t="n">
+      <c r="H7" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="24" t="e">
+      <c r="I7" s="23" t="e">
         <f aca="false">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8" t="n">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="n">
         <v>42324</v>
       </c>
-      <c r="H8" s="9" t="n">
+      <c r="H8" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="24" t="e">
+      <c r="I8" s="23" t="e">
         <f aca="false">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="8" t="n">
+      <c r="F9" s="24"/>
+      <c r="G9" s="7" t="n">
         <v>42338</v>
       </c>
-      <c r="H9" s="9" t="n">
+      <c r="H9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="24" t="e">
+      <c r="I9" s="23" t="e">
         <f aca="false">IF(AND(#REF!="Complete",#REF!=1),1,IF(ISBLANK(#REF!),2,IF(AND(#REF!&lt;&gt;"Complete",TODAY()&gt;#REF!),3,2)))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="0"/>
@@ -14611,79 +14613,79 @@
       <c r="J12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="29" t="n">
+      <c r="B14" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="31" t="n">
+      <c r="B15" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="29" t="n">
+      <c r="B16" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="31" t="n">
+      <c r="B17" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -14704,7 +14706,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8C8CFBB4-8731-4996-8625-D25EBE7E48D3}</x14:id>
+          <x14:id>{1FFC3D8A-29A0-4083-9581-305470FF9EC0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -14743,7 +14745,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8C8CFBB4-8731-4996-8625-D25EBE7E48D3}">
+          <x14:cfRule type="dataBar" id="{1FFC3D8A-29A0-4083-9581-305470FF9EC0}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic">
               <x14:cfvo type="autoMin" value="0"/>
               <x14:cfvo type="autoMax" value="0"/>
@@ -14777,7 +14779,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14787,17 +14789,17 @@
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14807,7 +14809,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>